<commit_message>
Add missing characteristics in the BioSamples brokering
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet2.xlsx
+++ b/tests/resources/brokering/metadata_sheet2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D829F24E-263D-2C4C-881B-62AE382A0175}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983B150B-6B6A-7346-B101-4327B0F09698}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -3026,6 +3026,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3035,23 +3050,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3431,8 +3431,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="82"/>
-      <c r="B1" s="82"/>
+      <c r="A1" s="76"/>
+      <c r="B1" s="76"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -3441,10 +3441,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83"/>
+      <c r="B2" s="77"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -3453,10 +3453,10 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="78" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3499,10 +3499,10 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="77"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3511,8 +3511,8 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -3543,10 +3543,10 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="84" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="84"/>
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="20">
       <c r="A12" s="35" t="s">
@@ -3599,28 +3599,28 @@
     </row>
     <row r="18" spans="1:2" s="11" customFormat="1"/>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="76"/>
+      <c r="B19" s="81"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="76"/>
+      <c r="B20" s="81"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="76"/>
+      <c r="B21" s="81"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="76"/>
+      <c r="B22" s="81"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1">
       <c r="A23" s="14"/>
@@ -3629,11 +3629,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3643,6 +3638,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3654,7 +3654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7144,8 +7144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
restore support for submission contact
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet2.xlsx
+++ b/tests/resources/brokering/metadata_sheet2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983B150B-6B6A-7346-B101-4327B0F09698}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16380441-8EE6-3946-9A3C-20FDE31562F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="767">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2471,6 +2471,15 @@
   </si>
   <si>
     <t>john.doe@example.com</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>jane.doe@example.com</t>
+  </si>
+  <si>
+    <t>TPTB</t>
   </si>
 </sst>
 </file>
@@ -3026,21 +3035,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3050,8 +3044,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3431,8 +3440,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="82"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -3441,10 +3450,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="77"/>
+      <c r="B2" s="83"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -3453,10 +3462,10 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="84" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="78"/>
+      <c r="B3" s="84"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3499,10 +3508,10 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="82"/>
+      <c r="B7" s="77"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3511,8 +3520,8 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1">
-      <c r="A8" s="83"/>
-      <c r="B8" s="83"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -3543,10 +3552,10 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="81" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="84"/>
+      <c r="B11" s="81"/>
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="20">
       <c r="A12" s="35" t="s">
@@ -3599,28 +3608,28 @@
     </row>
     <row r="18" spans="1:2" s="11" customFormat="1"/>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="81"/>
+      <c r="B19" s="76"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="81"/>
+      <c r="B20" s="76"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="81"/>
+      <c r="B21" s="76"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="81"/>
+      <c r="B22" s="76"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1">
       <c r="A23" s="14"/>
@@ -3629,6 +3638,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3638,11 +3652,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5409,10 +5418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -5467,9 +5476,32 @@
         <v>554</v>
       </c>
       <c r="F2" t="s">
+        <v>766</v>
+      </c>
+      <c r="G2" t="s">
         <v>556</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>764</v>
+      </c>
+      <c r="B3" t="s">
+        <v>761</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>762</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>765</v>
+      </c>
+      <c r="E3" t="s">
+        <v>554</v>
+      </c>
+      <c r="F3" t="s">
+        <v>766</v>
+      </c>
+      <c r="G3" t="s">
         <v>556</v>
       </c>
     </row>
@@ -5477,6 +5509,7 @@
   <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{D5EAB0F1-DA5A-1D43-AF07-384247652EC2}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5642,7 +5675,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7144,7 +7177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add a serialisation method to the mapping between metadata and biosample to convert dates to text. Update tests
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet2.xlsx
+++ b/tests/resources/brokering/metadata_sheet2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16380441-8EE6-3946-9A3C-20FDE31562F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48765435-9871-F346-8455-1D9A2A0B4633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40240" yWindow="1340" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -3035,6 +3035,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3044,23 +3059,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3440,8 +3440,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="82"/>
-      <c r="B1" s="82"/>
+      <c r="A1" s="76"/>
+      <c r="B1" s="76"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -3450,10 +3450,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83"/>
+      <c r="B2" s="77"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -3462,10 +3462,10 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="78" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3508,10 +3508,10 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="77"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3520,8 +3520,8 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -3552,10 +3552,10 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="84" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="84"/>
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="20">
       <c r="A12" s="35" t="s">
@@ -3608,28 +3608,28 @@
     </row>
     <row r="18" spans="1:2" s="11" customFormat="1"/>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="76"/>
+      <c r="B19" s="81"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="76"/>
+      <c r="B20" s="81"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="76"/>
+      <c r="B21" s="81"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="76"/>
+      <c r="B22" s="81"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1">
       <c r="A23" s="14"/>
@@ -3638,11 +3638,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3652,6 +3647,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5420,7 +5420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -7177,8 +7177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="M70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M103" sqref="M103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7499,6 +7499,9 @@
       <c r="M4" t="s">
         <v>548</v>
       </c>
+      <c r="AA4" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="5" spans="1:46">
       <c r="A5" t="s">
@@ -7516,6 +7519,9 @@
       <c r="M5" t="s">
         <v>548</v>
       </c>
+      <c r="AA5" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="6" spans="1:46">
       <c r="A6" t="s">
@@ -7533,6 +7539,9 @@
       <c r="M6" t="s">
         <v>548</v>
       </c>
+      <c r="AA6" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="7" spans="1:46">
       <c r="A7" t="s">
@@ -7551,6 +7560,9 @@
         <v>548</v>
       </c>
       <c r="Z7" s="72"/>
+      <c r="AA7" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="8" spans="1:46">
       <c r="A8" t="s">
@@ -7568,6 +7580,9 @@
       <c r="M8" t="s">
         <v>548</v>
       </c>
+      <c r="AA8" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="9" spans="1:46">
       <c r="A9" t="s">
@@ -7585,6 +7600,9 @@
       <c r="M9" t="s">
         <v>548</v>
       </c>
+      <c r="AA9" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="10" spans="1:46">
       <c r="A10" t="s">
@@ -7602,6 +7620,9 @@
       <c r="M10" t="s">
         <v>548</v>
       </c>
+      <c r="AA10" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="11" spans="1:46">
       <c r="A11" t="s">
@@ -7619,6 +7640,9 @@
       <c r="M11" t="s">
         <v>548</v>
       </c>
+      <c r="AA11" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="12" spans="1:46">
       <c r="A12" t="s">
@@ -7636,6 +7660,9 @@
       <c r="M12" t="s">
         <v>548</v>
       </c>
+      <c r="AA12" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="13" spans="1:46">
       <c r="A13" t="s">
@@ -7653,6 +7680,9 @@
       <c r="M13" t="s">
         <v>548</v>
       </c>
+      <c r="AA13" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="14" spans="1:46">
       <c r="A14" t="s">
@@ -7670,6 +7700,9 @@
       <c r="M14" t="s">
         <v>548</v>
       </c>
+      <c r="AA14" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="15" spans="1:46">
       <c r="A15" t="s">
@@ -7687,6 +7720,9 @@
       <c r="M15" t="s">
         <v>548</v>
       </c>
+      <c r="AA15" s="42">
+        <v>43845</v>
+      </c>
     </row>
     <row r="16" spans="1:46">
       <c r="A16" t="s">
@@ -7704,8 +7740,11 @@
       <c r="M16" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="AA16" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27">
       <c r="A17" t="s">
         <v>558</v>
       </c>
@@ -7721,8 +7760,11 @@
       <c r="M17" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="AA17" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27">
       <c r="A18" t="s">
         <v>558</v>
       </c>
@@ -7738,8 +7780,11 @@
       <c r="M18" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="AA18" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
       <c r="A19" t="s">
         <v>558</v>
       </c>
@@ -7755,8 +7800,11 @@
       <c r="M19" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="AA19" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
       <c r="A20" t="s">
         <v>558</v>
       </c>
@@ -7772,8 +7820,11 @@
       <c r="M20" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="AA20" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27">
       <c r="A21" t="s">
         <v>558</v>
       </c>
@@ -7789,8 +7840,11 @@
       <c r="M21" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="AA21" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27">
       <c r="A22" t="s">
         <v>558</v>
       </c>
@@ -7806,8 +7860,11 @@
       <c r="M22" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="AA22" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
       <c r="A23" t="s">
         <v>558</v>
       </c>
@@ -7823,8 +7880,11 @@
       <c r="M23" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="AA23" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
       <c r="A24" t="s">
         <v>558</v>
       </c>
@@ -7840,8 +7900,11 @@
       <c r="M24" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="AA24" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
       <c r="A25" t="s">
         <v>558</v>
       </c>
@@ -7857,8 +7920,11 @@
       <c r="M25" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="AA25" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
       <c r="A26" t="s">
         <v>558</v>
       </c>
@@ -7874,8 +7940,11 @@
       <c r="M26" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="AA26" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27">
       <c r="A27" t="s">
         <v>558</v>
       </c>
@@ -7891,8 +7960,11 @@
       <c r="M27" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="AA27" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27">
       <c r="A28" t="s">
         <v>558</v>
       </c>
@@ -7908,8 +7980,11 @@
       <c r="M28" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="AA28" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27">
       <c r="A29" t="s">
         <v>558</v>
       </c>
@@ -7925,8 +8000,11 @@
       <c r="M29" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="AA29" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27">
       <c r="A30" t="s">
         <v>558</v>
       </c>
@@ -7942,8 +8020,11 @@
       <c r="M30" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="AA30" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
       <c r="A31" t="s">
         <v>558</v>
       </c>
@@ -7959,8 +8040,11 @@
       <c r="M31" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="AA31" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27">
       <c r="A32" t="s">
         <v>558</v>
       </c>
@@ -7976,8 +8060,11 @@
       <c r="M32" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="AA32" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27">
       <c r="A33" t="s">
         <v>558</v>
       </c>
@@ -7993,8 +8080,11 @@
       <c r="M33" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="AA33" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27">
       <c r="A34" t="s">
         <v>558</v>
       </c>
@@ -8010,8 +8100,11 @@
       <c r="M34" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="AA34" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27">
       <c r="A35" t="s">
         <v>558</v>
       </c>
@@ -8027,8 +8120,11 @@
       <c r="M35" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="AA35" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27">
       <c r="A36" t="s">
         <v>558</v>
       </c>
@@ -8044,8 +8140,11 @@
       <c r="M36" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="AA36" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27">
       <c r="A37" t="s">
         <v>558</v>
       </c>
@@ -8061,8 +8160,11 @@
       <c r="M37" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="AA37" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27">
       <c r="A38" t="s">
         <v>558</v>
       </c>
@@ -8078,8 +8180,11 @@
       <c r="M38" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="AA38" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
       <c r="A39" t="s">
         <v>558</v>
       </c>
@@ -8095,8 +8200,11 @@
       <c r="M39" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="AA39" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27">
       <c r="A40" t="s">
         <v>558</v>
       </c>
@@ -8112,8 +8220,11 @@
       <c r="M40" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="AA40" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27">
       <c r="A41" t="s">
         <v>558</v>
       </c>
@@ -8129,8 +8240,11 @@
       <c r="M41" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="AA41" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27">
       <c r="A42" t="s">
         <v>558</v>
       </c>
@@ -8146,8 +8260,11 @@
       <c r="M42" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="AA42" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27">
       <c r="A43" t="s">
         <v>558</v>
       </c>
@@ -8163,8 +8280,11 @@
       <c r="M43" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="AA43" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27">
       <c r="A44" t="s">
         <v>558</v>
       </c>
@@ -8180,8 +8300,11 @@
       <c r="M44" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="AA44" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27">
       <c r="A45" t="s">
         <v>558</v>
       </c>
@@ -8197,8 +8320,11 @@
       <c r="M45" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="AA45" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27">
       <c r="A46" t="s">
         <v>558</v>
       </c>
@@ -8214,8 +8340,11 @@
       <c r="M46" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="AA46" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>558</v>
       </c>
@@ -8231,8 +8360,11 @@
       <c r="M47" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="AA47" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27">
       <c r="A48" t="s">
         <v>558</v>
       </c>
@@ -8248,8 +8380,11 @@
       <c r="M48" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="AA48" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27">
       <c r="A49" t="s">
         <v>558</v>
       </c>
@@ -8265,8 +8400,11 @@
       <c r="M49" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="AA49" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27">
       <c r="A50" t="s">
         <v>558</v>
       </c>
@@ -8282,8 +8420,11 @@
       <c r="M50" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="AA50" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27">
       <c r="A51" t="s">
         <v>558</v>
       </c>
@@ -8299,8 +8440,11 @@
       <c r="M51" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="AA51" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27">
       <c r="A52" t="s">
         <v>558</v>
       </c>
@@ -8316,8 +8460,11 @@
       <c r="M52" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="AA52" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27">
       <c r="A53" t="s">
         <v>558</v>
       </c>
@@ -8333,8 +8480,11 @@
       <c r="M53" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="AA53" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27">
       <c r="A54" t="s">
         <v>558</v>
       </c>
@@ -8350,8 +8500,11 @@
       <c r="M54" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="AA54" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27">
       <c r="A55" t="s">
         <v>558</v>
       </c>
@@ -8367,8 +8520,11 @@
       <c r="M55" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="AA55" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27">
       <c r="A56" t="s">
         <v>558</v>
       </c>
@@ -8384,8 +8540,11 @@
       <c r="M56" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="AA56" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27">
       <c r="A57" t="s">
         <v>558</v>
       </c>
@@ -8401,8 +8560,11 @@
       <c r="M57" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="AA57" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27">
       <c r="A58" t="s">
         <v>558</v>
       </c>
@@ -8418,8 +8580,11 @@
       <c r="M58" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="AA58" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27">
       <c r="A59" t="s">
         <v>558</v>
       </c>
@@ -8435,8 +8600,11 @@
       <c r="M59" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="AA59" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27">
       <c r="A60" t="s">
         <v>558</v>
       </c>
@@ -8452,8 +8620,11 @@
       <c r="M60" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="AA60" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27">
       <c r="A61" t="s">
         <v>558</v>
       </c>
@@ -8469,8 +8640,11 @@
       <c r="M61" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="AA61" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27">
       <c r="A62" t="s">
         <v>558</v>
       </c>
@@ -8486,8 +8660,11 @@
       <c r="M62" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="AA62" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27">
       <c r="A63" t="s">
         <v>558</v>
       </c>
@@ -8503,8 +8680,11 @@
       <c r="M63" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="AA63" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27">
       <c r="A64" t="s">
         <v>558</v>
       </c>
@@ -8520,8 +8700,11 @@
       <c r="M64" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="AA64" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27">
       <c r="A65" t="s">
         <v>558</v>
       </c>
@@ -8537,8 +8720,11 @@
       <c r="M65" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="AA65" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27">
       <c r="A66" t="s">
         <v>558</v>
       </c>
@@ -8554,8 +8740,11 @@
       <c r="M66" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="AA66" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27">
       <c r="A67" t="s">
         <v>558</v>
       </c>
@@ -8571,8 +8760,11 @@
       <c r="M67" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="AA67" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27">
       <c r="A68" t="s">
         <v>558</v>
       </c>
@@ -8588,8 +8780,11 @@
       <c r="M68" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="AA68" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27">
       <c r="A69" t="s">
         <v>558</v>
       </c>
@@ -8605,8 +8800,11 @@
       <c r="M69" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="AA69" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27">
       <c r="A70" t="s">
         <v>558</v>
       </c>
@@ -8622,8 +8820,11 @@
       <c r="M70" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="AA70" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27">
       <c r="A71" t="s">
         <v>558</v>
       </c>
@@ -8639,8 +8840,11 @@
       <c r="M71" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="AA71" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27">
       <c r="A72" t="s">
         <v>558</v>
       </c>
@@ -8656,8 +8860,11 @@
       <c r="M72" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="AA72" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27">
       <c r="A73" t="s">
         <v>558</v>
       </c>
@@ -8673,8 +8880,11 @@
       <c r="M73" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="AA73" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27">
       <c r="A74" t="s">
         <v>558</v>
       </c>
@@ -8690,8 +8900,11 @@
       <c r="M74" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="AA74" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27">
       <c r="A75" t="s">
         <v>558</v>
       </c>
@@ -8707,8 +8920,11 @@
       <c r="M75" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="AA75" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27">
       <c r="A76" t="s">
         <v>558</v>
       </c>
@@ -8724,8 +8940,11 @@
       <c r="M76" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="AA76" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27">
       <c r="A77" t="s">
         <v>558</v>
       </c>
@@ -8741,8 +8960,11 @@
       <c r="M77" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="AA77" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27">
       <c r="A78" t="s">
         <v>558</v>
       </c>
@@ -8758,8 +8980,11 @@
       <c r="M78" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="AA78" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27">
       <c r="A79" t="s">
         <v>558</v>
       </c>
@@ -8775,8 +9000,11 @@
       <c r="M79" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="AA79" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27">
       <c r="A80" t="s">
         <v>558</v>
       </c>
@@ -8792,8 +9020,11 @@
       <c r="M80" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="AA80" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
         <v>558</v>
       </c>
@@ -8809,8 +9040,11 @@
       <c r="M81" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="AA81" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
         <v>558</v>
       </c>
@@ -8826,8 +9060,11 @@
       <c r="M82" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="AA82" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
         <v>558</v>
       </c>
@@ -8843,8 +9080,11 @@
       <c r="M83" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="AA83" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
         <v>558</v>
       </c>
@@ -8860,8 +9100,11 @@
       <c r="M84" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="AA84" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
         <v>558</v>
       </c>
@@ -8877,8 +9120,11 @@
       <c r="M85" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="AA85" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27">
       <c r="A86" t="s">
         <v>558</v>
       </c>
@@ -8894,8 +9140,11 @@
       <c r="M86" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="AA86" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27">
       <c r="A87" t="s">
         <v>558</v>
       </c>
@@ -8911,8 +9160,11 @@
       <c r="M87" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="AA87" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27">
       <c r="A88" t="s">
         <v>558</v>
       </c>
@@ -8928,8 +9180,11 @@
       <c r="M88" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="AA88" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27">
       <c r="A89" t="s">
         <v>558</v>
       </c>
@@ -8945,8 +9200,11 @@
       <c r="M89" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="AA89" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
         <v>558</v>
       </c>
@@ -8962,8 +9220,11 @@
       <c r="M90" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="AA90" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
         <v>558</v>
       </c>
@@ -8979,8 +9240,11 @@
       <c r="M91" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="AA91" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
         <v>558</v>
       </c>
@@ -8996,8 +9260,11 @@
       <c r="M92" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="AA92" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
         <v>558</v>
       </c>
@@ -9013,8 +9280,11 @@
       <c r="M93" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="AA93" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
         <v>558</v>
       </c>
@@ -9030,8 +9300,11 @@
       <c r="M94" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="95" spans="1:13">
+      <c r="AA94" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
         <v>558</v>
       </c>
@@ -9047,8 +9320,11 @@
       <c r="M95" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="AA95" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
         <v>558</v>
       </c>
@@ -9064,8 +9340,11 @@
       <c r="M96" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="AA96" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="97" spans="1:27">
       <c r="A97" t="s">
         <v>558</v>
       </c>
@@ -9081,8 +9360,11 @@
       <c r="M97" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="AA97" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="98" spans="1:27">
       <c r="A98" t="s">
         <v>558</v>
       </c>
@@ -9098,8 +9380,11 @@
       <c r="M98" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="AA98" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27">
       <c r="A99" t="s">
         <v>558</v>
       </c>
@@ -9115,8 +9400,11 @@
       <c r="M99" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="AA99" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27">
       <c r="A100" t="s">
         <v>558</v>
       </c>
@@ -9132,8 +9420,11 @@
       <c r="M100" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="AA100" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27">
       <c r="A101" t="s">
         <v>558</v>
       </c>
@@ -9149,8 +9440,11 @@
       <c r="M101" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="AA101" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="102" spans="1:27">
       <c r="A102" t="s">
         <v>558</v>
       </c>
@@ -9166,8 +9460,11 @@
       <c r="M102" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="AA102" s="42">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="103" spans="1:27">
       <c r="A103" t="s">
         <v>558</v>
       </c>
@@ -9182,6 +9479,9 @@
       </c>
       <c r="M103" t="s">
         <v>548</v>
+      </c>
+      <c r="AA103" s="42">
+        <v>43845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make collection date and geo location Mandatory. Add default value in biosample brokering
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet2.xlsx
+++ b/tests/resources/brokering/metadata_sheet2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48765435-9871-F346-8455-1D9A2A0B4633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CECB4B9-460A-7E49-A573-3736DCAC05D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40240" yWindow="1340" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="767">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2892,19 +2892,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2913,25 +2912,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2940,23 +2931,14 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2966,7 +2948,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2985,8 +2967,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3008,59 +2989,54 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3068,7 +3044,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3426,7 +3402,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AMK23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -3436,208 +3412,216 @@
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="255.5" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.83203125" style="2" customWidth="1"/>
+    <col min="3" max="1025" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="77" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1">
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A3" s="78" t="s">
+      <c r="B2" s="69"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A3" s="70" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" s="9" customFormat="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" ht="19">
-      <c r="A6" s="7" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1">
+      <c r="A5" s="67"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A6" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="82" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A7" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1">
-      <c r="A8" s="83"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" ht="19">
-      <c r="A9" s="79" t="s">
+      <c r="B7" s="64"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1">
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A9" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" s="9" customFormat="1">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" s="11" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="84" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1">
+      <c r="A10" s="67"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A11" s="68" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="84"/>
-    </row>
-    <row r="12" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A12" s="35" t="s">
+      <c r="B11" s="68"/>
+    </row>
+    <row r="12" spans="1:8" ht="20">
+      <c r="A12" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A13" s="37" t="s">
+    <row r="13" spans="1:8" ht="20">
+      <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A14" s="38" t="s">
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" ht="20">
+      <c r="A14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="11" customFormat="1" ht="40">
-      <c r="A15" s="39" t="s">
+    <row r="15" spans="1:8" ht="40">
+      <c r="A15" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" ht="40">
-      <c r="A16" s="40" t="s">
+    <row r="16" spans="1:8" ht="40">
+      <c r="A16" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="11" customFormat="1" ht="20">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:2" ht="20">
+      <c r="A17" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="8" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="11" customFormat="1"/>
+    <row r="18" spans="1:2">
+      <c r="A18"/>
+      <c r="B18"/>
+    </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="81"/>
+      <c r="B19" s="63"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="81"/>
+      <c r="B20" s="63"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="81"/>
+      <c r="B21" s="63"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="81"/>
-    </row>
-    <row r="23" spans="1:2" s="4" customFormat="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="B22" s="63"/>
+    </row>
+    <row r="23" spans="1:2" s="3" customFormat="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3647,11 +3631,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3677,16 +3656,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3752,7 +3731,7 @@
   <sheetPr>
     <tabColor rgb="FFB3A2C7"/>
   </sheetPr>
-  <dimension ref="A1:K281"/>
+  <dimension ref="A1:G281"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3768,41 +3747,39 @@
     <col min="8" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="33" customFormat="1">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:7" s="20" customFormat="1">
+      <c r="A1" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>162</v>
       </c>
       <c r="E2" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="18" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>220</v>
       </c>
       <c r="B3" t="s">
@@ -3814,12 +3791,12 @@
       <c r="E3" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="24"/>
       <c r="G3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -3836,7 +3813,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>227</v>
       </c>
@@ -3850,7 +3827,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>230</v>
       </c>
@@ -3864,7 +3841,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>233</v>
       </c>
@@ -3878,7 +3855,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>236</v>
       </c>
@@ -3892,7 +3869,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>240</v>
       </c>
@@ -3906,7 +3883,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -3917,7 +3894,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>244</v>
       </c>
@@ -3928,7 +3905,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>246</v>
       </c>
@@ -3939,7 +3916,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>248</v>
       </c>
@@ -3947,7 +3924,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:7">
       <c r="B14" t="s">
         <v>249</v>
       </c>
@@ -3955,7 +3932,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:7">
       <c r="B15" t="s">
         <v>250</v>
       </c>
@@ -3963,7 +3940,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>251</v>
       </c>
@@ -4111,7 +4088,7 @@
       <c r="B34" t="s">
         <v>269</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4175,7 +4152,7 @@
       <c r="B42" t="s">
         <v>277</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4268,7 +4245,7 @@
       <c r="B54" t="s">
         <v>289</v>
       </c>
-      <c r="E54" s="33"/>
+      <c r="E54" s="20"/>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" t="s">
@@ -5436,26 +5413,26 @@
     <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="64" customFormat="1">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="33" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5466,10 +5443,10 @@
       <c r="B2" t="s">
         <v>761</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="60" t="s">
         <v>762</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="61" t="s">
         <v>763</v>
       </c>
       <c r="E2" t="s">
@@ -5489,10 +5466,10 @@
       <c r="B3" t="s">
         <v>761</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="60" t="s">
         <v>762</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="61" t="s">
         <v>765</v>
       </c>
       <c r="E3" t="s">
@@ -5535,50 +5512,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5618,7 +5595,7 @@
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5655,10 +5632,10 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="14" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5690,62 +5667,62 @@
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="40.5" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="42" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="32" customWidth="1"/>
     <col min="12" max="12" width="64.6640625" customWidth="1"/>
     <col min="13" max="14" width="6" customWidth="1"/>
     <col min="15" max="15" width="6.6640625" customWidth="1"/>
     <col min="16" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="64" customFormat="1">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="37" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="62" t="s">
         <v>553</v>
       </c>
       <c r="B2" t="s">
@@ -5788,15 +5765,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B2" t="s">
@@ -5804,7 +5781,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
@@ -5812,7 +5789,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
@@ -5820,7 +5797,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
@@ -5828,7 +5805,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>162</v>
       </c>
       <c r="B6" t="s">
@@ -5836,7 +5813,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="11" t="s">
         <v>163</v>
       </c>
       <c r="B7" t="s">
@@ -5860,7 +5837,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" t="s">
         <v>168</v>
       </c>
       <c r="B10" t="s">
@@ -5916,7 +5893,7 @@
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="11" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6081,7 +6058,7 @@
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="18" t="s">
+      <c r="A53" t="s">
         <v>187</v>
       </c>
     </row>
@@ -6121,7 +6098,7 @@
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="18" t="s">
+      <c r="A61" t="s">
         <v>191</v>
       </c>
     </row>
@@ -6185,7 +6162,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -6210,56 +6187,55 @@
     <col min="16" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="P1" s="64"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="75" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="62" t="s">
         <v>557</v>
       </c>
       <c r="B2" t="s">
@@ -6268,7 +6244,7 @@
       <c r="C2" t="s">
         <v>559</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="62" t="s">
         <v>553</v>
       </c>
       <c r="E2" t="s">
@@ -6278,7 +6254,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1"/>
+    <row r="3" spans="1:15" ht="15" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="1">
@@ -6318,850 +6294,438 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="2" width="212" style="18" customWidth="1"/>
+    <col min="2" max="2" width="212" customWidth="1"/>
     <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="57" customHeight="1">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:2" ht="57" customHeight="1">
+      <c r="A3" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="16" t="s">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="18"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="25" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="11" t="s">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12">
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" ht="17">
-      <c r="A15" s="25" t="s">
+      <c r="B14" s="16"/>
+    </row>
+    <row r="15" spans="1:2" ht="17">
+      <c r="A15" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="25" t="s">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="11" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="26" t="s">
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="11" t="s">
+      <c r="B18" s="16"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="11" t="s">
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="26" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="11" t="s">
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="11" t="s">
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="11" t="s">
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="11" t="s">
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="11" t="s">
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="26" t="s">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="11" t="s">
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="11" t="s">
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="11" t="s">
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="26" t="s">
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="11" t="s">
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="11" t="s">
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="11" t="s">
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="11" t="s">
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="11" t="s">
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
         <v>115</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="11" t="s">
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="11" t="s">
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="11" t="s">
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="11" t="s">
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:12" ht="51">
-      <c r="A41" s="11" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="51">
+      <c r="A41" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="26" t="s">
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="11" t="s">
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="11" t="s">
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="11" t="s">
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46" s="11" t="s">
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
         <v>134</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="11" t="s">
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
         <v>136</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="11" t="s">
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="11" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="B49" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50" s="11" t="s">
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="11" t="s">
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>144</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="A52" s="11" t="s">
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>146</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" s="26" t="s">
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="1:12" ht="24">
-      <c r="A54" s="30" t="s">
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:2" ht="24">
+      <c r="A54" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-    </row>
-    <row r="55" spans="1:12" ht="15" customHeight="1">
-      <c r="A55" s="31" t="s">
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:2" ht="15" customHeight="1">
+      <c r="A55" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="A56" s="11" t="s">
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="16" t="s">
         <v>152</v>
       </c>
     </row>
@@ -7177,8 +6741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M103" sqref="M103"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7207,7 +6771,7 @@
     <col min="23" max="23" width="11.5" customWidth="1"/>
     <col min="24" max="24" width="15.6640625" customWidth="1"/>
     <col min="25" max="26" width="16.6640625" customWidth="1"/>
-    <col min="27" max="27" width="13.83203125" style="42" customWidth="1"/>
+    <col min="27" max="27" width="13.83203125" style="32" customWidth="1"/>
     <col min="28" max="28" width="34.33203125" customWidth="1"/>
     <col min="29" max="29" width="33.6640625" customWidth="1"/>
     <col min="30" max="30" width="4.6640625" customWidth="1"/>
@@ -7230,256 +6794,256 @@
     <col min="47" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="65" customFormat="1">
-      <c r="A1" s="62"/>
-      <c r="B1" s="86" t="s">
+    <row r="1" spans="1:46">
+      <c r="A1" s="51"/>
+      <c r="B1" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="49" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="68"/>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="69"/>
-    </row>
-    <row r="2" spans="1:46" s="64" customFormat="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="85" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="55"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="55"/>
+      <c r="AG1" s="55"/>
+      <c r="AH1" s="55"/>
+      <c r="AI1" s="55"/>
+      <c r="AJ1" s="55"/>
+      <c r="AK1" s="55"/>
+      <c r="AL1" s="55"/>
+      <c r="AM1" s="55"/>
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="55"/>
+      <c r="AS1" s="55"/>
+      <c r="AT1" s="56"/>
+    </row>
+    <row r="2" spans="1:46">
+      <c r="A2" s="52"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="88" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88" t="s">
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="85" t="s">
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85" t="s">
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="X2" s="85"/>
-      <c r="Y2" s="85"/>
-      <c r="Z2" s="85" t="s">
+      <c r="X2" s="71"/>
+      <c r="Y2" s="71"/>
+      <c r="Z2" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="85"/>
-      <c r="AC2" s="85"/>
-      <c r="AD2" s="85"/>
-      <c r="AE2" s="85"/>
-      <c r="AF2" s="85"/>
-      <c r="AG2" s="85"/>
-      <c r="AH2" s="85"/>
-      <c r="AI2" s="85"/>
-      <c r="AJ2" s="85" t="s">
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="71"/>
+      <c r="AI2" s="71"/>
+      <c r="AJ2" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="AK2" s="85"/>
-      <c r="AL2" s="85"/>
-      <c r="AM2" s="85"/>
-      <c r="AN2" s="85"/>
-      <c r="AO2" s="85"/>
-      <c r="AP2" s="85"/>
-      <c r="AQ2" s="85"/>
-      <c r="AR2" s="85"/>
-      <c r="AS2" s="85"/>
-    </row>
-    <row r="3" spans="1:46" s="64" customFormat="1" ht="26">
-      <c r="A3" s="50" t="s">
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="71"/>
+      <c r="AR2" s="71"/>
+      <c r="AS2" s="71"/>
+    </row>
+    <row r="3" spans="1:46" ht="26">
+      <c r="A3" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="58" t="s">
+      <c r="N3" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="O3" s="57" t="s">
+      <c r="O3" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="P3" s="59" t="s">
+      <c r="P3" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="Q3" s="57" t="s">
+      <c r="Q3" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="R3" s="60" t="s">
+      <c r="R3" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="57" t="s">
+      <c r="S3" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="57" t="s">
+      <c r="T3" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="57" t="s">
+      <c r="U3" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="V3" s="58" t="s">
+      <c r="V3" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="W3" s="60" t="s">
+      <c r="W3" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="X3" s="57" t="s">
+      <c r="X3" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="Y3" s="58" t="s">
+      <c r="Y3" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="Z3" s="60" t="s">
+      <c r="Z3" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="AA3" s="71" t="s">
+      <c r="AA3" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="AB3" s="57" t="s">
+      <c r="AB3" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="57" t="s">
+      <c r="AC3" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="AD3" s="57" t="s">
+      <c r="AD3" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="AE3" s="57" t="s">
+      <c r="AE3" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="AF3" s="57" t="s">
+      <c r="AF3" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="AG3" s="57" t="s">
+      <c r="AG3" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="AH3" s="57" t="s">
+      <c r="AH3" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="AI3" s="58" t="s">
+      <c r="AI3" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="AJ3" s="60" t="s">
+      <c r="AJ3" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="AK3" s="57" t="s">
+      <c r="AK3" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="AL3" s="57" t="s">
+      <c r="AL3" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="AM3" s="57" t="s">
+      <c r="AM3" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="AN3" s="57" t="s">
+      <c r="AN3" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="AO3" s="57" t="s">
+      <c r="AO3" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="AP3" s="57" t="s">
+      <c r="AP3" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="AQ3" s="57" t="s">
+      <c r="AQ3" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="AR3" s="57" t="s">
+      <c r="AR3" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="AS3" s="58" t="s">
+      <c r="AS3" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="AT3" s="61" t="s">
+      <c r="AT3" s="50" t="s">
         <v>148</v>
       </c>
     </row>
@@ -7499,8 +7063,11 @@
       <c r="M4" t="s">
         <v>548</v>
       </c>
-      <c r="AA4" s="42">
-        <v>43845</v>
+      <c r="AA4" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:46">
@@ -7519,8 +7086,11 @@
       <c r="M5" t="s">
         <v>548</v>
       </c>
-      <c r="AA5" s="42">
-        <v>43845</v>
+      <c r="AA5" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:46">
@@ -7539,8 +7109,11 @@
       <c r="M6" t="s">
         <v>548</v>
       </c>
-      <c r="AA6" s="42">
-        <v>43845</v>
+      <c r="AA6" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:46">
@@ -7559,9 +7132,12 @@
       <c r="M7" t="s">
         <v>548</v>
       </c>
-      <c r="Z7" s="72"/>
-      <c r="AA7" s="42">
-        <v>43845</v>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="8" spans="1:46">
@@ -7580,8 +7156,11 @@
       <c r="M8" t="s">
         <v>548</v>
       </c>
-      <c r="AA8" s="42">
-        <v>43845</v>
+      <c r="AA8" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:46">
@@ -7600,8 +7179,11 @@
       <c r="M9" t="s">
         <v>548</v>
       </c>
-      <c r="AA9" s="42">
-        <v>43845</v>
+      <c r="AA9" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="1:46">
@@ -7620,8 +7202,11 @@
       <c r="M10" t="s">
         <v>548</v>
       </c>
-      <c r="AA10" s="42">
-        <v>43845</v>
+      <c r="AA10" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:46">
@@ -7640,8 +7225,11 @@
       <c r="M11" t="s">
         <v>548</v>
       </c>
-      <c r="AA11" s="42">
-        <v>43845</v>
+      <c r="AA11" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:46">
@@ -7660,8 +7248,11 @@
       <c r="M12" t="s">
         <v>548</v>
       </c>
-      <c r="AA12" s="42">
-        <v>43845</v>
+      <c r="AA12" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="13" spans="1:46">
@@ -7680,8 +7271,11 @@
       <c r="M13" t="s">
         <v>548</v>
       </c>
-      <c r="AA13" s="42">
-        <v>43845</v>
+      <c r="AA13" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="14" spans="1:46">
@@ -7700,8 +7294,11 @@
       <c r="M14" t="s">
         <v>548</v>
       </c>
-      <c r="AA14" s="42">
-        <v>43845</v>
+      <c r="AA14" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="15" spans="1:46">
@@ -7720,8 +7317,11 @@
       <c r="M15" t="s">
         <v>548</v>
       </c>
-      <c r="AA15" s="42">
-        <v>43845</v>
+      <c r="AA15" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="16" spans="1:46">
@@ -7740,11 +7340,14 @@
       <c r="M16" t="s">
         <v>548</v>
       </c>
-      <c r="AA16" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
+      <c r="AA16" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
         <v>558</v>
       </c>
@@ -7760,11 +7363,14 @@
       <c r="M17" t="s">
         <v>548</v>
       </c>
-      <c r="AA17" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27">
+      <c r="AA17" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
         <v>558</v>
       </c>
@@ -7780,11 +7386,14 @@
       <c r="M18" t="s">
         <v>548</v>
       </c>
-      <c r="AA18" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27">
+      <c r="AA18" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>558</v>
       </c>
@@ -7800,11 +7409,14 @@
       <c r="M19" t="s">
         <v>548</v>
       </c>
-      <c r="AA19" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+      <c r="AA19" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>558</v>
       </c>
@@ -7820,11 +7432,14 @@
       <c r="M20" t="s">
         <v>548</v>
       </c>
-      <c r="AA20" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
+      <c r="AA20" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>558</v>
       </c>
@@ -7840,11 +7455,14 @@
       <c r="M21" t="s">
         <v>548</v>
       </c>
-      <c r="AA21" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
+      <c r="AA21" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28">
       <c r="A22" t="s">
         <v>558</v>
       </c>
@@ -7860,11 +7478,14 @@
       <c r="M22" t="s">
         <v>548</v>
       </c>
-      <c r="AA22" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
+      <c r="AA22" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28">
       <c r="A23" t="s">
         <v>558</v>
       </c>
@@ -7880,11 +7501,14 @@
       <c r="M23" t="s">
         <v>548</v>
       </c>
-      <c r="AA23" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27">
+      <c r="AA23" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28">
       <c r="A24" t="s">
         <v>558</v>
       </c>
@@ -7900,11 +7524,14 @@
       <c r="M24" t="s">
         <v>548</v>
       </c>
-      <c r="AA24" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
+      <c r="AA24" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28">
       <c r="A25" t="s">
         <v>558</v>
       </c>
@@ -7920,11 +7547,14 @@
       <c r="M25" t="s">
         <v>548</v>
       </c>
-      <c r="AA25" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27">
+      <c r="AA25" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28">
       <c r="A26" t="s">
         <v>558</v>
       </c>
@@ -7940,11 +7570,14 @@
       <c r="M26" t="s">
         <v>548</v>
       </c>
-      <c r="AA26" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27">
+      <c r="AA26" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28">
       <c r="A27" t="s">
         <v>558</v>
       </c>
@@ -7960,11 +7593,14 @@
       <c r="M27" t="s">
         <v>548</v>
       </c>
-      <c r="AA27" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27">
+      <c r="AA27" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28">
       <c r="A28" t="s">
         <v>558</v>
       </c>
@@ -7980,11 +7616,14 @@
       <c r="M28" t="s">
         <v>548</v>
       </c>
-      <c r="AA28" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27">
+      <c r="AA28" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
       <c r="A29" t="s">
         <v>558</v>
       </c>
@@ -8000,11 +7639,14 @@
       <c r="M29" t="s">
         <v>548</v>
       </c>
-      <c r="AA29" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27">
+      <c r="AA29" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28">
       <c r="A30" t="s">
         <v>558</v>
       </c>
@@ -8020,11 +7662,14 @@
       <c r="M30" t="s">
         <v>548</v>
       </c>
-      <c r="AA30" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27">
+      <c r="AA30" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28">
       <c r="A31" t="s">
         <v>558</v>
       </c>
@@ -8040,11 +7685,14 @@
       <c r="M31" t="s">
         <v>548</v>
       </c>
-      <c r="AA31" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27">
+      <c r="AA31" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28">
       <c r="A32" t="s">
         <v>558</v>
       </c>
@@ -8060,11 +7708,14 @@
       <c r="M32" t="s">
         <v>548</v>
       </c>
-      <c r="AA32" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27">
+      <c r="AA32" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28">
       <c r="A33" t="s">
         <v>558</v>
       </c>
@@ -8080,11 +7731,14 @@
       <c r="M33" t="s">
         <v>548</v>
       </c>
-      <c r="AA33" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27">
+      <c r="AA33" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28">
       <c r="A34" t="s">
         <v>558</v>
       </c>
@@ -8100,11 +7754,14 @@
       <c r="M34" t="s">
         <v>548</v>
       </c>
-      <c r="AA34" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
+      <c r="AA34" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28">
       <c r="A35" t="s">
         <v>558</v>
       </c>
@@ -8120,11 +7777,14 @@
       <c r="M35" t="s">
         <v>548</v>
       </c>
-      <c r="AA35" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27">
+      <c r="AA35" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28">
       <c r="A36" t="s">
         <v>558</v>
       </c>
@@ -8140,11 +7800,14 @@
       <c r="M36" t="s">
         <v>548</v>
       </c>
-      <c r="AA36" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27">
+      <c r="AA36" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28">
       <c r="A37" t="s">
         <v>558</v>
       </c>
@@ -8160,11 +7823,14 @@
       <c r="M37" t="s">
         <v>548</v>
       </c>
-      <c r="AA37" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27">
+      <c r="AA37" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28">
       <c r="A38" t="s">
         <v>558</v>
       </c>
@@ -8180,11 +7846,14 @@
       <c r="M38" t="s">
         <v>548</v>
       </c>
-      <c r="AA38" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27">
+      <c r="AA38" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28">
       <c r="A39" t="s">
         <v>558</v>
       </c>
@@ -8200,11 +7869,14 @@
       <c r="M39" t="s">
         <v>548</v>
       </c>
-      <c r="AA39" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27">
+      <c r="AA39" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28">
       <c r="A40" t="s">
         <v>558</v>
       </c>
@@ -8220,11 +7892,14 @@
       <c r="M40" t="s">
         <v>548</v>
       </c>
-      <c r="AA40" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27">
+      <c r="AA40" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
       <c r="A41" t="s">
         <v>558</v>
       </c>
@@ -8240,11 +7915,14 @@
       <c r="M41" t="s">
         <v>548</v>
       </c>
-      <c r="AA41" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27">
+      <c r="AA41" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28">
       <c r="A42" t="s">
         <v>558</v>
       </c>
@@ -8260,11 +7938,14 @@
       <c r="M42" t="s">
         <v>548</v>
       </c>
-      <c r="AA42" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27">
+      <c r="AA42" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
       <c r="A43" t="s">
         <v>558</v>
       </c>
@@ -8280,11 +7961,14 @@
       <c r="M43" t="s">
         <v>548</v>
       </c>
-      <c r="AA43" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27">
+      <c r="AA43" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
       <c r="A44" t="s">
         <v>558</v>
       </c>
@@ -8300,11 +7984,14 @@
       <c r="M44" t="s">
         <v>548</v>
       </c>
-      <c r="AA44" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27">
+      <c r="AA44" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
       <c r="A45" t="s">
         <v>558</v>
       </c>
@@ -8320,11 +8007,14 @@
       <c r="M45" t="s">
         <v>548</v>
       </c>
-      <c r="AA45" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27">
+      <c r="AA45" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
       <c r="A46" t="s">
         <v>558</v>
       </c>
@@ -8340,11 +8030,14 @@
       <c r="M46" t="s">
         <v>548</v>
       </c>
-      <c r="AA46" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27">
+      <c r="AA46" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
       <c r="A47" t="s">
         <v>558</v>
       </c>
@@ -8360,11 +8053,14 @@
       <c r="M47" t="s">
         <v>548</v>
       </c>
-      <c r="AA47" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27">
+      <c r="AA47" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28">
       <c r="A48" t="s">
         <v>558</v>
       </c>
@@ -8380,11 +8076,14 @@
       <c r="M48" t="s">
         <v>548</v>
       </c>
-      <c r="AA48" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27">
+      <c r="AA48" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28">
       <c r="A49" t="s">
         <v>558</v>
       </c>
@@ -8400,11 +8099,14 @@
       <c r="M49" t="s">
         <v>548</v>
       </c>
-      <c r="AA49" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27">
+      <c r="AA49" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28">
       <c r="A50" t="s">
         <v>558</v>
       </c>
@@ -8420,11 +8122,14 @@
       <c r="M50" t="s">
         <v>548</v>
       </c>
-      <c r="AA50" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="51" spans="1:27">
+      <c r="AA50" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28">
       <c r="A51" t="s">
         <v>558</v>
       </c>
@@ -8440,11 +8145,14 @@
       <c r="M51" t="s">
         <v>548</v>
       </c>
-      <c r="AA51" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="52" spans="1:27">
+      <c r="AA51" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28">
       <c r="A52" t="s">
         <v>558</v>
       </c>
@@ -8460,11 +8168,14 @@
       <c r="M52" t="s">
         <v>548</v>
       </c>
-      <c r="AA52" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="53" spans="1:27">
+      <c r="AA52" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28">
       <c r="A53" t="s">
         <v>558</v>
       </c>
@@ -8480,11 +8191,14 @@
       <c r="M53" t="s">
         <v>548</v>
       </c>
-      <c r="AA53" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="54" spans="1:27">
+      <c r="AA53" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28">
       <c r="A54" t="s">
         <v>558</v>
       </c>
@@ -8500,11 +8214,14 @@
       <c r="M54" t="s">
         <v>548</v>
       </c>
-      <c r="AA54" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="55" spans="1:27">
+      <c r="AA54" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28">
       <c r="A55" t="s">
         <v>558</v>
       </c>
@@ -8520,11 +8237,14 @@
       <c r="M55" t="s">
         <v>548</v>
       </c>
-      <c r="AA55" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="56" spans="1:27">
+      <c r="AA55" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28">
       <c r="A56" t="s">
         <v>558</v>
       </c>
@@ -8540,11 +8260,14 @@
       <c r="M56" t="s">
         <v>548</v>
       </c>
-      <c r="AA56" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27">
+      <c r="AA56" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28">
       <c r="A57" t="s">
         <v>558</v>
       </c>
@@ -8560,11 +8283,14 @@
       <c r="M57" t="s">
         <v>548</v>
       </c>
-      <c r="AA57" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="58" spans="1:27">
+      <c r="AA57" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28">
       <c r="A58" t="s">
         <v>558</v>
       </c>
@@ -8580,11 +8306,14 @@
       <c r="M58" t="s">
         <v>548</v>
       </c>
-      <c r="AA58" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27">
+      <c r="AA58" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28">
       <c r="A59" t="s">
         <v>558</v>
       </c>
@@ -8600,11 +8329,14 @@
       <c r="M59" t="s">
         <v>548</v>
       </c>
-      <c r="AA59" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27">
+      <c r="AA59" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28">
       <c r="A60" t="s">
         <v>558</v>
       </c>
@@ -8620,11 +8352,14 @@
       <c r="M60" t="s">
         <v>548</v>
       </c>
-      <c r="AA60" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27">
+      <c r="AA60" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28">
       <c r="A61" t="s">
         <v>558</v>
       </c>
@@ -8640,11 +8375,14 @@
       <c r="M61" t="s">
         <v>548</v>
       </c>
-      <c r="AA61" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27">
+      <c r="AA61" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28">
       <c r="A62" t="s">
         <v>558</v>
       </c>
@@ -8660,11 +8398,14 @@
       <c r="M62" t="s">
         <v>548</v>
       </c>
-      <c r="AA62" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="63" spans="1:27">
+      <c r="AA62" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28">
       <c r="A63" t="s">
         <v>558</v>
       </c>
@@ -8680,11 +8421,14 @@
       <c r="M63" t="s">
         <v>548</v>
       </c>
-      <c r="AA63" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="64" spans="1:27">
+      <c r="AA63" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28">
       <c r="A64" t="s">
         <v>558</v>
       </c>
@@ -8700,11 +8444,14 @@
       <c r="M64" t="s">
         <v>548</v>
       </c>
-      <c r="AA64" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="65" spans="1:27">
+      <c r="AA64" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28">
       <c r="A65" t="s">
         <v>558</v>
       </c>
@@ -8720,11 +8467,14 @@
       <c r="M65" t="s">
         <v>548</v>
       </c>
-      <c r="AA65" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="66" spans="1:27">
+      <c r="AA65" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28">
       <c r="A66" t="s">
         <v>558</v>
       </c>
@@ -8740,11 +8490,14 @@
       <c r="M66" t="s">
         <v>548</v>
       </c>
-      <c r="AA66" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="67" spans="1:27">
+      <c r="AA66" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28">
       <c r="A67" t="s">
         <v>558</v>
       </c>
@@ -8760,11 +8513,14 @@
       <c r="M67" t="s">
         <v>548</v>
       </c>
-      <c r="AA67" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="68" spans="1:27">
+      <c r="AA67" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28">
       <c r="A68" t="s">
         <v>558</v>
       </c>
@@ -8780,11 +8536,14 @@
       <c r="M68" t="s">
         <v>548</v>
       </c>
-      <c r="AA68" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="69" spans="1:27">
+      <c r="AA68" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28">
       <c r="A69" t="s">
         <v>558</v>
       </c>
@@ -8800,11 +8559,14 @@
       <c r="M69" t="s">
         <v>548</v>
       </c>
-      <c r="AA69" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="70" spans="1:27">
+      <c r="AA69" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28">
       <c r="A70" t="s">
         <v>558</v>
       </c>
@@ -8820,11 +8582,14 @@
       <c r="M70" t="s">
         <v>548</v>
       </c>
-      <c r="AA70" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="71" spans="1:27">
+      <c r="AA70" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28">
       <c r="A71" t="s">
         <v>558</v>
       </c>
@@ -8840,11 +8605,14 @@
       <c r="M71" t="s">
         <v>548</v>
       </c>
-      <c r="AA71" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="72" spans="1:27">
+      <c r="AA71" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28">
       <c r="A72" t="s">
         <v>558</v>
       </c>
@@ -8860,11 +8628,14 @@
       <c r="M72" t="s">
         <v>548</v>
       </c>
-      <c r="AA72" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="73" spans="1:27">
+      <c r="AA72" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28">
       <c r="A73" t="s">
         <v>558</v>
       </c>
@@ -8880,11 +8651,14 @@
       <c r="M73" t="s">
         <v>548</v>
       </c>
-      <c r="AA73" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="74" spans="1:27">
+      <c r="AA73" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28">
       <c r="A74" t="s">
         <v>558</v>
       </c>
@@ -8900,11 +8674,14 @@
       <c r="M74" t="s">
         <v>548</v>
       </c>
-      <c r="AA74" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="75" spans="1:27">
+      <c r="AA74" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28">
       <c r="A75" t="s">
         <v>558</v>
       </c>
@@ -8920,11 +8697,14 @@
       <c r="M75" t="s">
         <v>548</v>
       </c>
-      <c r="AA75" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="76" spans="1:27">
+      <c r="AA75" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28">
       <c r="A76" t="s">
         <v>558</v>
       </c>
@@ -8940,11 +8720,14 @@
       <c r="M76" t="s">
         <v>548</v>
       </c>
-      <c r="AA76" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="77" spans="1:27">
+      <c r="AA76" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28">
       <c r="A77" t="s">
         <v>558</v>
       </c>
@@ -8960,11 +8743,14 @@
       <c r="M77" t="s">
         <v>548</v>
       </c>
-      <c r="AA77" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="78" spans="1:27">
+      <c r="AA77" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28">
       <c r="A78" t="s">
         <v>558</v>
       </c>
@@ -8980,11 +8766,14 @@
       <c r="M78" t="s">
         <v>548</v>
       </c>
-      <c r="AA78" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="79" spans="1:27">
+      <c r="AA78" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28">
       <c r="A79" t="s">
         <v>558</v>
       </c>
@@ -9000,11 +8789,14 @@
       <c r="M79" t="s">
         <v>548</v>
       </c>
-      <c r="AA79" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="80" spans="1:27">
+      <c r="AA79" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28">
       <c r="A80" t="s">
         <v>558</v>
       </c>
@@ -9020,11 +8812,14 @@
       <c r="M80" t="s">
         <v>548</v>
       </c>
-      <c r="AA80" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="81" spans="1:27">
+      <c r="AA80" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28">
       <c r="A81" t="s">
         <v>558</v>
       </c>
@@ -9040,11 +8835,14 @@
       <c r="M81" t="s">
         <v>548</v>
       </c>
-      <c r="AA81" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="82" spans="1:27">
+      <c r="AA81" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28">
       <c r="A82" t="s">
         <v>558</v>
       </c>
@@ -9060,11 +8858,14 @@
       <c r="M82" t="s">
         <v>548</v>
       </c>
-      <c r="AA82" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="83" spans="1:27">
+      <c r="AA82" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28">
       <c r="A83" t="s">
         <v>558</v>
       </c>
@@ -9080,11 +8881,14 @@
       <c r="M83" t="s">
         <v>548</v>
       </c>
-      <c r="AA83" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="84" spans="1:27">
+      <c r="AA83" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28">
       <c r="A84" t="s">
         <v>558</v>
       </c>
@@ -9100,11 +8904,14 @@
       <c r="M84" t="s">
         <v>548</v>
       </c>
-      <c r="AA84" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="85" spans="1:27">
+      <c r="AA84" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28">
       <c r="A85" t="s">
         <v>558</v>
       </c>
@@ -9120,11 +8927,14 @@
       <c r="M85" t="s">
         <v>548</v>
       </c>
-      <c r="AA85" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="86" spans="1:27">
+      <c r="AA85" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28">
       <c r="A86" t="s">
         <v>558</v>
       </c>
@@ -9140,11 +8950,14 @@
       <c r="M86" t="s">
         <v>548</v>
       </c>
-      <c r="AA86" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="87" spans="1:27">
+      <c r="AA86" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28">
       <c r="A87" t="s">
         <v>558</v>
       </c>
@@ -9160,11 +8973,14 @@
       <c r="M87" t="s">
         <v>548</v>
       </c>
-      <c r="AA87" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="88" spans="1:27">
+      <c r="AA87" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB87" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28">
       <c r="A88" t="s">
         <v>558</v>
       </c>
@@ -9180,11 +8996,14 @@
       <c r="M88" t="s">
         <v>548</v>
       </c>
-      <c r="AA88" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="89" spans="1:27">
+      <c r="AA88" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB88" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28">
       <c r="A89" t="s">
         <v>558</v>
       </c>
@@ -9200,11 +9019,14 @@
       <c r="M89" t="s">
         <v>548</v>
       </c>
-      <c r="AA89" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="90" spans="1:27">
+      <c r="AA89" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB89" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28">
       <c r="A90" t="s">
         <v>558</v>
       </c>
@@ -9220,11 +9042,14 @@
       <c r="M90" t="s">
         <v>548</v>
       </c>
-      <c r="AA90" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="91" spans="1:27">
+      <c r="AA90" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB90" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28">
       <c r="A91" t="s">
         <v>558</v>
       </c>
@@ -9240,11 +9065,14 @@
       <c r="M91" t="s">
         <v>548</v>
       </c>
-      <c r="AA91" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="92" spans="1:27">
+      <c r="AA91" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB91" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28">
       <c r="A92" t="s">
         <v>558</v>
       </c>
@@ -9260,11 +9088,14 @@
       <c r="M92" t="s">
         <v>548</v>
       </c>
-      <c r="AA92" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="93" spans="1:27">
+      <c r="AA92" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB92" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28">
       <c r="A93" t="s">
         <v>558</v>
       </c>
@@ -9280,11 +9111,14 @@
       <c r="M93" t="s">
         <v>548</v>
       </c>
-      <c r="AA93" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="94" spans="1:27">
+      <c r="AA93" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB93" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28">
       <c r="A94" t="s">
         <v>558</v>
       </c>
@@ -9300,11 +9134,14 @@
       <c r="M94" t="s">
         <v>548</v>
       </c>
-      <c r="AA94" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="95" spans="1:27">
+      <c r="AA94" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB94" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28">
       <c r="A95" t="s">
         <v>558</v>
       </c>
@@ -9320,11 +9157,14 @@
       <c r="M95" t="s">
         <v>548</v>
       </c>
-      <c r="AA95" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="96" spans="1:27">
+      <c r="AA95" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB95" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28">
       <c r="A96" t="s">
         <v>558</v>
       </c>
@@ -9340,11 +9180,14 @@
       <c r="M96" t="s">
         <v>548</v>
       </c>
-      <c r="AA96" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="97" spans="1:27">
+      <c r="AA96" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB96" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28">
       <c r="A97" t="s">
         <v>558</v>
       </c>
@@ -9360,11 +9203,14 @@
       <c r="M97" t="s">
         <v>548</v>
       </c>
-      <c r="AA97" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="98" spans="1:27">
+      <c r="AA97" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB97" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28">
       <c r="A98" t="s">
         <v>558</v>
       </c>
@@ -9380,11 +9226,14 @@
       <c r="M98" t="s">
         <v>548</v>
       </c>
-      <c r="AA98" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="99" spans="1:27">
+      <c r="AA98" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB98" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28">
       <c r="A99" t="s">
         <v>558</v>
       </c>
@@ -9400,11 +9249,14 @@
       <c r="M99" t="s">
         <v>548</v>
       </c>
-      <c r="AA99" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="100" spans="1:27">
+      <c r="AA99" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB99" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28">
       <c r="A100" t="s">
         <v>558</v>
       </c>
@@ -9420,11 +9272,14 @@
       <c r="M100" t="s">
         <v>548</v>
       </c>
-      <c r="AA100" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="101" spans="1:27">
+      <c r="AA100" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28">
       <c r="A101" t="s">
         <v>558</v>
       </c>
@@ -9440,11 +9295,14 @@
       <c r="M101" t="s">
         <v>548</v>
       </c>
-      <c r="AA101" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="102" spans="1:27">
+      <c r="AA101" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB101" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28">
       <c r="A102" t="s">
         <v>558</v>
       </c>
@@ -9460,11 +9318,14 @@
       <c r="M102" t="s">
         <v>548</v>
       </c>
-      <c r="AA102" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="103" spans="1:27">
+      <c r="AA102" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB102" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28">
       <c r="A103" t="s">
         <v>558</v>
       </c>
@@ -9480,8 +9341,11 @@
       <c r="M103" t="s">
         <v>548</v>
       </c>
-      <c r="AA103" s="42">
-        <v>43845</v>
+      <c r="AA103" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB103" t="s">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -9554,15 +9418,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
@@ -9570,7 +9434,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>215</v>
       </c>
       <c r="B3" t="s">
@@ -9578,7 +9442,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>217</v>
       </c>
       <c r="B4" t="s">
@@ -9586,7 +9450,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="11" t="s">
         <v>218</v>
       </c>
       <c r="B5" t="s">

</xml_diff>

<commit_message>
improve the novel attributes validation
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet2.xlsx
+++ b/tests/resources/brokering/metadata_sheet2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48765435-9871-F346-8455-1D9A2A0B4633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDF1A7E-EA45-A14E-B10B-BE9532D677E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40240" yWindow="1340" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Files" sheetId="10" r:id="rId10"/>
     <sheet name="CVs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="768">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2481,6 +2481,9 @@
   <si>
     <t>TPTB</t>
   </si>
+  <si>
+    <t>BL_w_tail:39.0,BL_wo_tail:19.0,bmi_wo_tail:7.14681440443213,bmi_w_tail:1.69625246548323,weight:258.0</t>
+  </si>
 </sst>
 </file>
 
@@ -2489,7 +2492,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2667,6 +2670,13 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2892,19 +2902,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2913,25 +2922,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2940,23 +2941,14 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2966,7 +2958,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2985,8 +2977,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3008,55 +2999,50 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3068,12 +3054,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3426,7 +3413,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AMK23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -3436,204 +3423,207 @@
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="255.5" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.83203125" style="2" customWidth="1"/>
+    <col min="3" max="1025" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="77" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1">
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A3" s="78" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A3" s="65" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" s="9" customFormat="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" ht="19">
-      <c r="A6" s="7" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1">
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A6" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="82" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A7" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1">
-      <c r="A8" s="83"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" ht="19">
-      <c r="A9" s="79" t="s">
+      <c r="B7" s="68"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1">
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A9" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" s="9" customFormat="1">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" s="11" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="84" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1">
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A11" s="70" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="84"/>
-    </row>
-    <row r="12" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A12" s="35" t="s">
+      <c r="B11" s="70"/>
+    </row>
+    <row r="12" spans="1:8" ht="20">
+      <c r="A12" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A13" s="37" t="s">
+    <row r="13" spans="1:8" ht="20">
+      <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A14" s="38" t="s">
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" ht="20">
+      <c r="A14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="11" customFormat="1" ht="40">
-      <c r="A15" s="39" t="s">
+    <row r="15" spans="1:8" ht="40">
+      <c r="A15" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" ht="40">
-      <c r="A16" s="40" t="s">
+    <row r="16" spans="1:8" ht="40">
+      <c r="A16" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="11" customFormat="1" ht="20">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:2" ht="20">
+      <c r="A17" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="8" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="11" customFormat="1"/>
+    <row r="18" spans="1:2">
+      <c r="A18"/>
+      <c r="B18"/>
+    </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="81"/>
+      <c r="B19" s="67"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="81"/>
+      <c r="B20" s="67"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="81"/>
+      <c r="B21" s="67"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="81"/>
-    </row>
-    <row r="23" spans="1:2" s="4" customFormat="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="B22" s="67"/>
+    </row>
+    <row r="23" spans="1:2" s="3" customFormat="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -3677,16 +3667,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3752,7 +3742,7 @@
   <sheetPr>
     <tabColor rgb="FFB3A2C7"/>
   </sheetPr>
-  <dimension ref="A1:K281"/>
+  <dimension ref="A1:G281"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3768,41 +3758,39 @@
     <col min="8" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="33" customFormat="1">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:7" s="20" customFormat="1">
+      <c r="A1" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>162</v>
       </c>
       <c r="E2" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="18" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>220</v>
       </c>
       <c r="B3" t="s">
@@ -3814,12 +3802,12 @@
       <c r="E3" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="24"/>
       <c r="G3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -3836,7 +3824,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>227</v>
       </c>
@@ -3850,7 +3838,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>230</v>
       </c>
@@ -3864,7 +3852,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>233</v>
       </c>
@@ -3878,7 +3866,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>236</v>
       </c>
@@ -3892,7 +3880,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>240</v>
       </c>
@@ -3906,7 +3894,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -3917,7 +3905,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>244</v>
       </c>
@@ -3928,7 +3916,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>246</v>
       </c>
@@ -3939,7 +3927,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>248</v>
       </c>
@@ -3947,7 +3935,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:7">
       <c r="B14" t="s">
         <v>249</v>
       </c>
@@ -3955,7 +3943,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:7">
       <c r="B15" t="s">
         <v>250</v>
       </c>
@@ -3963,7 +3951,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>251</v>
       </c>
@@ -4111,7 +4099,7 @@
       <c r="B34" t="s">
         <v>269</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4175,7 +4163,7 @@
       <c r="B42" t="s">
         <v>277</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4268,7 +4256,7 @@
       <c r="B54" t="s">
         <v>289</v>
       </c>
-      <c r="E54" s="33"/>
+      <c r="E54" s="20"/>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" t="s">
@@ -5436,26 +5424,26 @@
     <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="64" customFormat="1">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="33" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5466,10 +5454,10 @@
       <c r="B2" t="s">
         <v>761</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="60" t="s">
         <v>762</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="61" t="s">
         <v>763</v>
       </c>
       <c r="E2" t="s">
@@ -5489,10 +5477,10 @@
       <c r="B3" t="s">
         <v>761</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="60" t="s">
         <v>762</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="61" t="s">
         <v>765</v>
       </c>
       <c r="E3" t="s">
@@ -5535,50 +5523,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5618,7 +5606,7 @@
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5655,10 +5643,10 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="14" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5690,62 +5678,62 @@
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="40.5" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="42" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="32" customWidth="1"/>
     <col min="12" max="12" width="64.6640625" customWidth="1"/>
     <col min="13" max="14" width="6" customWidth="1"/>
     <col min="15" max="15" width="6.6640625" customWidth="1"/>
     <col min="16" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="64" customFormat="1">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="37" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="62" t="s">
         <v>553</v>
       </c>
       <c r="B2" t="s">
@@ -5788,15 +5776,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B2" t="s">
@@ -5804,7 +5792,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
@@ -5812,7 +5800,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
@@ -5820,7 +5808,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
@@ -5828,7 +5816,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>162</v>
       </c>
       <c r="B6" t="s">
@@ -5836,7 +5824,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="11" t="s">
         <v>163</v>
       </c>
       <c r="B7" t="s">
@@ -5860,7 +5848,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" t="s">
         <v>168</v>
       </c>
       <c r="B10" t="s">
@@ -5916,7 +5904,7 @@
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="11" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6081,7 +6069,7 @@
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="18" t="s">
+      <c r="A53" t="s">
         <v>187</v>
       </c>
     </row>
@@ -6121,7 +6109,7 @@
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="18" t="s">
+      <c r="A61" t="s">
         <v>191</v>
       </c>
     </row>
@@ -6185,7 +6173,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -6210,56 +6198,55 @@
     <col min="16" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="P1" s="64"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="75" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="62" t="s">
         <v>557</v>
       </c>
       <c r="B2" t="s">
@@ -6268,7 +6255,7 @@
       <c r="C2" t="s">
         <v>559</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="62" t="s">
         <v>553</v>
       </c>
       <c r="E2" t="s">
@@ -6278,7 +6265,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1"/>
+    <row r="3" spans="1:15" ht="15" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="1">
@@ -6318,850 +6305,438 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="2" width="212" style="18" customWidth="1"/>
+    <col min="2" max="2" width="212" customWidth="1"/>
     <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="57" customHeight="1">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:2" ht="57" customHeight="1">
+      <c r="A3" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="16" t="s">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="18"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="25" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="11" t="s">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12">
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" ht="17">
-      <c r="A15" s="25" t="s">
+      <c r="B14" s="16"/>
+    </row>
+    <row r="15" spans="1:2" ht="17">
+      <c r="A15" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="25" t="s">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="11" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="26" t="s">
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="11" t="s">
+      <c r="B18" s="16"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="11" t="s">
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="26" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="11" t="s">
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="11" t="s">
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="11" t="s">
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="11" t="s">
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="11" t="s">
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="26" t="s">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="11" t="s">
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="11" t="s">
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="11" t="s">
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="26" t="s">
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="11" t="s">
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="11" t="s">
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="11" t="s">
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="11" t="s">
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="11" t="s">
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
         <v>115</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="11" t="s">
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="11" t="s">
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="11" t="s">
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="11" t="s">
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:12" ht="51">
-      <c r="A41" s="11" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="51">
+      <c r="A41" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="26" t="s">
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="11" t="s">
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="11" t="s">
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="11" t="s">
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46" s="11" t="s">
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
         <v>134</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="11" t="s">
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
         <v>136</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="11" t="s">
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="11" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="B49" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50" s="11" t="s">
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="11" t="s">
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>144</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="A52" s="11" t="s">
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>146</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" s="26" t="s">
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="1:12" ht="24">
-      <c r="A54" s="30" t="s">
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:2" ht="24">
+      <c r="A54" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-    </row>
-    <row r="55" spans="1:12" ht="15" customHeight="1">
-      <c r="A55" s="31" t="s">
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:2" ht="15" customHeight="1">
+      <c r="A55" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="A56" s="11" t="s">
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="16" t="s">
         <v>152</v>
       </c>
     </row>
@@ -7177,8 +6752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M103" sqref="M103"/>
+    <sheetView tabSelected="1" topLeftCell="AA3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT4" sqref="AT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7207,7 +6782,7 @@
     <col min="23" max="23" width="11.5" customWidth="1"/>
     <col min="24" max="24" width="15.6640625" customWidth="1"/>
     <col min="25" max="26" width="16.6640625" customWidth="1"/>
-    <col min="27" max="27" width="13.83203125" style="42" customWidth="1"/>
+    <col min="27" max="27" width="13.83203125" style="32" customWidth="1"/>
     <col min="28" max="28" width="34.33203125" customWidth="1"/>
     <col min="29" max="29" width="33.6640625" customWidth="1"/>
     <col min="30" max="30" width="4.6640625" customWidth="1"/>
@@ -7230,256 +6805,256 @@
     <col min="47" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="65" customFormat="1">
-      <c r="A1" s="62"/>
-      <c r="B1" s="86" t="s">
+    <row r="1" spans="1:46">
+      <c r="A1" s="51"/>
+      <c r="B1" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="49" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="68"/>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="69"/>
-    </row>
-    <row r="2" spans="1:46" s="64" customFormat="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="85" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="55"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="55"/>
+      <c r="AG1" s="55"/>
+      <c r="AH1" s="55"/>
+      <c r="AI1" s="55"/>
+      <c r="AJ1" s="55"/>
+      <c r="AK1" s="55"/>
+      <c r="AL1" s="55"/>
+      <c r="AM1" s="55"/>
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="55"/>
+      <c r="AS1" s="55"/>
+      <c r="AT1" s="56"/>
+    </row>
+    <row r="2" spans="1:46">
+      <c r="A2" s="52"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="88" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88" t="s">
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="85" t="s">
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85" t="s">
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="X2" s="85"/>
-      <c r="Y2" s="85"/>
-      <c r="Z2" s="85" t="s">
+      <c r="X2" s="71"/>
+      <c r="Y2" s="71"/>
+      <c r="Z2" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="85"/>
-      <c r="AC2" s="85"/>
-      <c r="AD2" s="85"/>
-      <c r="AE2" s="85"/>
-      <c r="AF2" s="85"/>
-      <c r="AG2" s="85"/>
-      <c r="AH2" s="85"/>
-      <c r="AI2" s="85"/>
-      <c r="AJ2" s="85" t="s">
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="71"/>
+      <c r="AI2" s="71"/>
+      <c r="AJ2" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="AK2" s="85"/>
-      <c r="AL2" s="85"/>
-      <c r="AM2" s="85"/>
-      <c r="AN2" s="85"/>
-      <c r="AO2" s="85"/>
-      <c r="AP2" s="85"/>
-      <c r="AQ2" s="85"/>
-      <c r="AR2" s="85"/>
-      <c r="AS2" s="85"/>
-    </row>
-    <row r="3" spans="1:46" s="64" customFormat="1" ht="26">
-      <c r="A3" s="50" t="s">
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="71"/>
+      <c r="AR2" s="71"/>
+      <c r="AS2" s="71"/>
+    </row>
+    <row r="3" spans="1:46" ht="26">
+      <c r="A3" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="58" t="s">
+      <c r="N3" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="O3" s="57" t="s">
+      <c r="O3" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="P3" s="59" t="s">
+      <c r="P3" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="Q3" s="57" t="s">
+      <c r="Q3" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="R3" s="60" t="s">
+      <c r="R3" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="57" t="s">
+      <c r="S3" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="57" t="s">
+      <c r="T3" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="57" t="s">
+      <c r="U3" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="V3" s="58" t="s">
+      <c r="V3" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="W3" s="60" t="s">
+      <c r="W3" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="X3" s="57" t="s">
+      <c r="X3" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="Y3" s="58" t="s">
+      <c r="Y3" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="Z3" s="60" t="s">
+      <c r="Z3" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="AA3" s="71" t="s">
+      <c r="AA3" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="AB3" s="57" t="s">
+      <c r="AB3" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="57" t="s">
+      <c r="AC3" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="AD3" s="57" t="s">
+      <c r="AD3" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="AE3" s="57" t="s">
+      <c r="AE3" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="AF3" s="57" t="s">
+      <c r="AF3" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="AG3" s="57" t="s">
+      <c r="AG3" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="AH3" s="57" t="s">
+      <c r="AH3" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="AI3" s="58" t="s">
+      <c r="AI3" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="AJ3" s="60" t="s">
+      <c r="AJ3" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="AK3" s="57" t="s">
+      <c r="AK3" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="AL3" s="57" t="s">
+      <c r="AL3" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="AM3" s="57" t="s">
+      <c r="AM3" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="AN3" s="57" t="s">
+      <c r="AN3" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="AO3" s="57" t="s">
+      <c r="AO3" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="AP3" s="57" t="s">
+      <c r="AP3" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="AQ3" s="57" t="s">
+      <c r="AQ3" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="AR3" s="57" t="s">
+      <c r="AR3" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="AS3" s="58" t="s">
+      <c r="AS3" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="AT3" s="61" t="s">
+      <c r="AT3" s="50" t="s">
         <v>148</v>
       </c>
     </row>
@@ -7499,8 +7074,14 @@
       <c r="M4" t="s">
         <v>548</v>
       </c>
-      <c r="AA4" s="42">
-        <v>43845</v>
+      <c r="AA4" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>515</v>
+      </c>
+      <c r="AT4" s="75" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="5" spans="1:46">
@@ -7519,8 +7100,11 @@
       <c r="M5" t="s">
         <v>548</v>
       </c>
-      <c r="AA5" s="42">
-        <v>43845</v>
+      <c r="AA5" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:46">
@@ -7539,8 +7123,11 @@
       <c r="M6" t="s">
         <v>548</v>
       </c>
-      <c r="AA6" s="42">
-        <v>43845</v>
+      <c r="AA6" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:46">
@@ -7559,9 +7146,12 @@
       <c r="M7" t="s">
         <v>548</v>
       </c>
-      <c r="Z7" s="72"/>
-      <c r="AA7" s="42">
-        <v>43845</v>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="8" spans="1:46">
@@ -7580,8 +7170,11 @@
       <c r="M8" t="s">
         <v>548</v>
       </c>
-      <c r="AA8" s="42">
-        <v>43845</v>
+      <c r="AA8" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:46">
@@ -7600,8 +7193,11 @@
       <c r="M9" t="s">
         <v>548</v>
       </c>
-      <c r="AA9" s="42">
-        <v>43845</v>
+      <c r="AA9" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="1:46">
@@ -7620,8 +7216,11 @@
       <c r="M10" t="s">
         <v>548</v>
       </c>
-      <c r="AA10" s="42">
-        <v>43845</v>
+      <c r="AA10" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:46">
@@ -7640,8 +7239,11 @@
       <c r="M11" t="s">
         <v>548</v>
       </c>
-      <c r="AA11" s="42">
-        <v>43845</v>
+      <c r="AA11" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:46">
@@ -7660,8 +7262,11 @@
       <c r="M12" t="s">
         <v>548</v>
       </c>
-      <c r="AA12" s="42">
-        <v>43845</v>
+      <c r="AA12" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="13" spans="1:46">
@@ -7680,8 +7285,11 @@
       <c r="M13" t="s">
         <v>548</v>
       </c>
-      <c r="AA13" s="42">
-        <v>43845</v>
+      <c r="AA13" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="14" spans="1:46">
@@ -7700,8 +7308,11 @@
       <c r="M14" t="s">
         <v>548</v>
       </c>
-      <c r="AA14" s="42">
-        <v>43845</v>
+      <c r="AA14" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="15" spans="1:46">
@@ -7720,8 +7331,11 @@
       <c r="M15" t="s">
         <v>548</v>
       </c>
-      <c r="AA15" s="42">
-        <v>43845</v>
+      <c r="AA15" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="16" spans="1:46">
@@ -7740,11 +7354,14 @@
       <c r="M16" t="s">
         <v>548</v>
       </c>
-      <c r="AA16" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
+      <c r="AA16" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
         <v>558</v>
       </c>
@@ -7760,11 +7377,14 @@
       <c r="M17" t="s">
         <v>548</v>
       </c>
-      <c r="AA17" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27">
+      <c r="AA17" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
         <v>558</v>
       </c>
@@ -7780,11 +7400,14 @@
       <c r="M18" t="s">
         <v>548</v>
       </c>
-      <c r="AA18" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27">
+      <c r="AA18" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>558</v>
       </c>
@@ -7800,11 +7423,14 @@
       <c r="M19" t="s">
         <v>548</v>
       </c>
-      <c r="AA19" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+      <c r="AA19" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>558</v>
       </c>
@@ -7820,11 +7446,14 @@
       <c r="M20" t="s">
         <v>548</v>
       </c>
-      <c r="AA20" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
+      <c r="AA20" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>558</v>
       </c>
@@ -7840,11 +7469,14 @@
       <c r="M21" t="s">
         <v>548</v>
       </c>
-      <c r="AA21" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
+      <c r="AA21" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28">
       <c r="A22" t="s">
         <v>558</v>
       </c>
@@ -7860,11 +7492,14 @@
       <c r="M22" t="s">
         <v>548</v>
       </c>
-      <c r="AA22" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
+      <c r="AA22" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28">
       <c r="A23" t="s">
         <v>558</v>
       </c>
@@ -7880,11 +7515,14 @@
       <c r="M23" t="s">
         <v>548</v>
       </c>
-      <c r="AA23" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27">
+      <c r="AA23" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28">
       <c r="A24" t="s">
         <v>558</v>
       </c>
@@ -7900,11 +7538,14 @@
       <c r="M24" t="s">
         <v>548</v>
       </c>
-      <c r="AA24" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
+      <c r="AA24" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28">
       <c r="A25" t="s">
         <v>558</v>
       </c>
@@ -7920,11 +7561,14 @@
       <c r="M25" t="s">
         <v>548</v>
       </c>
-      <c r="AA25" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27">
+      <c r="AA25" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28">
       <c r="A26" t="s">
         <v>558</v>
       </c>
@@ -7940,11 +7584,14 @@
       <c r="M26" t="s">
         <v>548</v>
       </c>
-      <c r="AA26" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27">
+      <c r="AA26" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28">
       <c r="A27" t="s">
         <v>558</v>
       </c>
@@ -7960,11 +7607,14 @@
       <c r="M27" t="s">
         <v>548</v>
       </c>
-      <c r="AA27" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27">
+      <c r="AA27" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28">
       <c r="A28" t="s">
         <v>558</v>
       </c>
@@ -7980,11 +7630,14 @@
       <c r="M28" t="s">
         <v>548</v>
       </c>
-      <c r="AA28" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27">
+      <c r="AA28" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
       <c r="A29" t="s">
         <v>558</v>
       </c>
@@ -8000,11 +7653,14 @@
       <c r="M29" t="s">
         <v>548</v>
       </c>
-      <c r="AA29" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27">
+      <c r="AA29" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28">
       <c r="A30" t="s">
         <v>558</v>
       </c>
@@ -8020,11 +7676,14 @@
       <c r="M30" t="s">
         <v>548</v>
       </c>
-      <c r="AA30" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27">
+      <c r="AA30" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28">
       <c r="A31" t="s">
         <v>558</v>
       </c>
@@ -8040,11 +7699,14 @@
       <c r="M31" t="s">
         <v>548</v>
       </c>
-      <c r="AA31" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27">
+      <c r="AA31" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28">
       <c r="A32" t="s">
         <v>558</v>
       </c>
@@ -8060,11 +7722,14 @@
       <c r="M32" t="s">
         <v>548</v>
       </c>
-      <c r="AA32" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27">
+      <c r="AA32" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28">
       <c r="A33" t="s">
         <v>558</v>
       </c>
@@ -8080,11 +7745,14 @@
       <c r="M33" t="s">
         <v>548</v>
       </c>
-      <c r="AA33" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27">
+      <c r="AA33" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28">
       <c r="A34" t="s">
         <v>558</v>
       </c>
@@ -8100,11 +7768,14 @@
       <c r="M34" t="s">
         <v>548</v>
       </c>
-      <c r="AA34" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
+      <c r="AA34" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28">
       <c r="A35" t="s">
         <v>558</v>
       </c>
@@ -8120,11 +7791,14 @@
       <c r="M35" t="s">
         <v>548</v>
       </c>
-      <c r="AA35" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27">
+      <c r="AA35" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28">
       <c r="A36" t="s">
         <v>558</v>
       </c>
@@ -8140,11 +7814,14 @@
       <c r="M36" t="s">
         <v>548</v>
       </c>
-      <c r="AA36" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27">
+      <c r="AA36" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28">
       <c r="A37" t="s">
         <v>558</v>
       </c>
@@ -8160,11 +7837,14 @@
       <c r="M37" t="s">
         <v>548</v>
       </c>
-      <c r="AA37" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27">
+      <c r="AA37" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28">
       <c r="A38" t="s">
         <v>558</v>
       </c>
@@ -8180,11 +7860,14 @@
       <c r="M38" t="s">
         <v>548</v>
       </c>
-      <c r="AA38" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27">
+      <c r="AA38" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28">
       <c r="A39" t="s">
         <v>558</v>
       </c>
@@ -8200,11 +7883,14 @@
       <c r="M39" t="s">
         <v>548</v>
       </c>
-      <c r="AA39" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27">
+      <c r="AA39" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28">
       <c r="A40" t="s">
         <v>558</v>
       </c>
@@ -8220,11 +7906,14 @@
       <c r="M40" t="s">
         <v>548</v>
       </c>
-      <c r="AA40" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27">
+      <c r="AA40" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
       <c r="A41" t="s">
         <v>558</v>
       </c>
@@ -8240,11 +7929,14 @@
       <c r="M41" t="s">
         <v>548</v>
       </c>
-      <c r="AA41" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27">
+      <c r="AA41" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28">
       <c r="A42" t="s">
         <v>558</v>
       </c>
@@ -8260,11 +7952,14 @@
       <c r="M42" t="s">
         <v>548</v>
       </c>
-      <c r="AA42" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27">
+      <c r="AA42" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
       <c r="A43" t="s">
         <v>558</v>
       </c>
@@ -8280,11 +7975,14 @@
       <c r="M43" t="s">
         <v>548</v>
       </c>
-      <c r="AA43" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27">
+      <c r="AA43" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
       <c r="A44" t="s">
         <v>558</v>
       </c>
@@ -8300,11 +7998,14 @@
       <c r="M44" t="s">
         <v>548</v>
       </c>
-      <c r="AA44" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27">
+      <c r="AA44" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
       <c r="A45" t="s">
         <v>558</v>
       </c>
@@ -8320,11 +8021,14 @@
       <c r="M45" t="s">
         <v>548</v>
       </c>
-      <c r="AA45" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27">
+      <c r="AA45" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
       <c r="A46" t="s">
         <v>558</v>
       </c>
@@ -8340,11 +8044,14 @@
       <c r="M46" t="s">
         <v>548</v>
       </c>
-      <c r="AA46" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27">
+      <c r="AA46" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
       <c r="A47" t="s">
         <v>558</v>
       </c>
@@ -8360,11 +8067,14 @@
       <c r="M47" t="s">
         <v>548</v>
       </c>
-      <c r="AA47" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27">
+      <c r="AA47" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28">
       <c r="A48" t="s">
         <v>558</v>
       </c>
@@ -8380,11 +8090,14 @@
       <c r="M48" t="s">
         <v>548</v>
       </c>
-      <c r="AA48" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27">
+      <c r="AA48" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28">
       <c r="A49" t="s">
         <v>558</v>
       </c>
@@ -8400,11 +8113,14 @@
       <c r="M49" t="s">
         <v>548</v>
       </c>
-      <c r="AA49" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27">
+      <c r="AA49" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28">
       <c r="A50" t="s">
         <v>558</v>
       </c>
@@ -8420,11 +8136,14 @@
       <c r="M50" t="s">
         <v>548</v>
       </c>
-      <c r="AA50" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="51" spans="1:27">
+      <c r="AA50" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28">
       <c r="A51" t="s">
         <v>558</v>
       </c>
@@ -8440,11 +8159,14 @@
       <c r="M51" t="s">
         <v>548</v>
       </c>
-      <c r="AA51" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="52" spans="1:27">
+      <c r="AA51" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28">
       <c r="A52" t="s">
         <v>558</v>
       </c>
@@ -8460,11 +8182,14 @@
       <c r="M52" t="s">
         <v>548</v>
       </c>
-      <c r="AA52" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="53" spans="1:27">
+      <c r="AA52" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28">
       <c r="A53" t="s">
         <v>558</v>
       </c>
@@ -8480,11 +8205,14 @@
       <c r="M53" t="s">
         <v>548</v>
       </c>
-      <c r="AA53" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="54" spans="1:27">
+      <c r="AA53" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28">
       <c r="A54" t="s">
         <v>558</v>
       </c>
@@ -8500,11 +8228,14 @@
       <c r="M54" t="s">
         <v>548</v>
       </c>
-      <c r="AA54" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="55" spans="1:27">
+      <c r="AA54" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28">
       <c r="A55" t="s">
         <v>558</v>
       </c>
@@ -8520,11 +8251,14 @@
       <c r="M55" t="s">
         <v>548</v>
       </c>
-      <c r="AA55" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="56" spans="1:27">
+      <c r="AA55" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28">
       <c r="A56" t="s">
         <v>558</v>
       </c>
@@ -8540,11 +8274,14 @@
       <c r="M56" t="s">
         <v>548</v>
       </c>
-      <c r="AA56" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27">
+      <c r="AA56" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28">
       <c r="A57" t="s">
         <v>558</v>
       </c>
@@ -8560,11 +8297,14 @@
       <c r="M57" t="s">
         <v>548</v>
       </c>
-      <c r="AA57" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="58" spans="1:27">
+      <c r="AA57" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28">
       <c r="A58" t="s">
         <v>558</v>
       </c>
@@ -8580,11 +8320,14 @@
       <c r="M58" t="s">
         <v>548</v>
       </c>
-      <c r="AA58" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27">
+      <c r="AA58" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28">
       <c r="A59" t="s">
         <v>558</v>
       </c>
@@ -8600,11 +8343,14 @@
       <c r="M59" t="s">
         <v>548</v>
       </c>
-      <c r="AA59" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27">
+      <c r="AA59" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28">
       <c r="A60" t="s">
         <v>558</v>
       </c>
@@ -8620,11 +8366,14 @@
       <c r="M60" t="s">
         <v>548</v>
       </c>
-      <c r="AA60" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27">
+      <c r="AA60" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28">
       <c r="A61" t="s">
         <v>558</v>
       </c>
@@ -8640,11 +8389,14 @@
       <c r="M61" t="s">
         <v>548</v>
       </c>
-      <c r="AA61" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27">
+      <c r="AA61" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28">
       <c r="A62" t="s">
         <v>558</v>
       </c>
@@ -8660,11 +8412,14 @@
       <c r="M62" t="s">
         <v>548</v>
       </c>
-      <c r="AA62" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="63" spans="1:27">
+      <c r="AA62" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28">
       <c r="A63" t="s">
         <v>558</v>
       </c>
@@ -8680,11 +8435,14 @@
       <c r="M63" t="s">
         <v>548</v>
       </c>
-      <c r="AA63" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="64" spans="1:27">
+      <c r="AA63" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28">
       <c r="A64" t="s">
         <v>558</v>
       </c>
@@ -8700,11 +8458,14 @@
       <c r="M64" t="s">
         <v>548</v>
       </c>
-      <c r="AA64" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="65" spans="1:27">
+      <c r="AA64" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28">
       <c r="A65" t="s">
         <v>558</v>
       </c>
@@ -8720,11 +8481,14 @@
       <c r="M65" t="s">
         <v>548</v>
       </c>
-      <c r="AA65" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="66" spans="1:27">
+      <c r="AA65" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28">
       <c r="A66" t="s">
         <v>558</v>
       </c>
@@ -8740,11 +8504,14 @@
       <c r="M66" t="s">
         <v>548</v>
       </c>
-      <c r="AA66" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="67" spans="1:27">
+      <c r="AA66" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28">
       <c r="A67" t="s">
         <v>558</v>
       </c>
@@ -8760,11 +8527,14 @@
       <c r="M67" t="s">
         <v>548</v>
       </c>
-      <c r="AA67" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="68" spans="1:27">
+      <c r="AA67" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28">
       <c r="A68" t="s">
         <v>558</v>
       </c>
@@ -8780,11 +8550,14 @@
       <c r="M68" t="s">
         <v>548</v>
       </c>
-      <c r="AA68" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="69" spans="1:27">
+      <c r="AA68" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28">
       <c r="A69" t="s">
         <v>558</v>
       </c>
@@ -8800,11 +8573,14 @@
       <c r="M69" t="s">
         <v>548</v>
       </c>
-      <c r="AA69" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="70" spans="1:27">
+      <c r="AA69" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28">
       <c r="A70" t="s">
         <v>558</v>
       </c>
@@ -8820,11 +8596,14 @@
       <c r="M70" t="s">
         <v>548</v>
       </c>
-      <c r="AA70" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="71" spans="1:27">
+      <c r="AA70" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28">
       <c r="A71" t="s">
         <v>558</v>
       </c>
@@ -8840,11 +8619,14 @@
       <c r="M71" t="s">
         <v>548</v>
       </c>
-      <c r="AA71" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="72" spans="1:27">
+      <c r="AA71" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28">
       <c r="A72" t="s">
         <v>558</v>
       </c>
@@ -8860,11 +8642,14 @@
       <c r="M72" t="s">
         <v>548</v>
       </c>
-      <c r="AA72" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="73" spans="1:27">
+      <c r="AA72" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28">
       <c r="A73" t="s">
         <v>558</v>
       </c>
@@ -8880,11 +8665,14 @@
       <c r="M73" t="s">
         <v>548</v>
       </c>
-      <c r="AA73" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="74" spans="1:27">
+      <c r="AA73" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28">
       <c r="A74" t="s">
         <v>558</v>
       </c>
@@ -8900,11 +8688,14 @@
       <c r="M74" t="s">
         <v>548</v>
       </c>
-      <c r="AA74" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="75" spans="1:27">
+      <c r="AA74" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28">
       <c r="A75" t="s">
         <v>558</v>
       </c>
@@ -8920,11 +8711,14 @@
       <c r="M75" t="s">
         <v>548</v>
       </c>
-      <c r="AA75" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="76" spans="1:27">
+      <c r="AA75" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28">
       <c r="A76" t="s">
         <v>558</v>
       </c>
@@ -8940,11 +8734,14 @@
       <c r="M76" t="s">
         <v>548</v>
       </c>
-      <c r="AA76" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="77" spans="1:27">
+      <c r="AA76" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28">
       <c r="A77" t="s">
         <v>558</v>
       </c>
@@ -8960,11 +8757,14 @@
       <c r="M77" t="s">
         <v>548</v>
       </c>
-      <c r="AA77" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="78" spans="1:27">
+      <c r="AA77" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28">
       <c r="A78" t="s">
         <v>558</v>
       </c>
@@ -8980,11 +8780,14 @@
       <c r="M78" t="s">
         <v>548</v>
       </c>
-      <c r="AA78" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="79" spans="1:27">
+      <c r="AA78" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28">
       <c r="A79" t="s">
         <v>558</v>
       </c>
@@ -9000,11 +8803,14 @@
       <c r="M79" t="s">
         <v>548</v>
       </c>
-      <c r="AA79" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="80" spans="1:27">
+      <c r="AA79" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28">
       <c r="A80" t="s">
         <v>558</v>
       </c>
@@ -9020,11 +8826,14 @@
       <c r="M80" t="s">
         <v>548</v>
       </c>
-      <c r="AA80" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="81" spans="1:27">
+      <c r="AA80" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28">
       <c r="A81" t="s">
         <v>558</v>
       </c>
@@ -9040,11 +8849,14 @@
       <c r="M81" t="s">
         <v>548</v>
       </c>
-      <c r="AA81" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="82" spans="1:27">
+      <c r="AA81" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28">
       <c r="A82" t="s">
         <v>558</v>
       </c>
@@ -9060,11 +8872,14 @@
       <c r="M82" t="s">
         <v>548</v>
       </c>
-      <c r="AA82" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="83" spans="1:27">
+      <c r="AA82" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28">
       <c r="A83" t="s">
         <v>558</v>
       </c>
@@ -9080,11 +8895,14 @@
       <c r="M83" t="s">
         <v>548</v>
       </c>
-      <c r="AA83" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="84" spans="1:27">
+      <c r="AA83" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28">
       <c r="A84" t="s">
         <v>558</v>
       </c>
@@ -9100,11 +8918,14 @@
       <c r="M84" t="s">
         <v>548</v>
       </c>
-      <c r="AA84" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="85" spans="1:27">
+      <c r="AA84" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28">
       <c r="A85" t="s">
         <v>558</v>
       </c>
@@ -9120,11 +8941,14 @@
       <c r="M85" t="s">
         <v>548</v>
       </c>
-      <c r="AA85" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="86" spans="1:27">
+      <c r="AA85" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28">
       <c r="A86" t="s">
         <v>558</v>
       </c>
@@ -9140,11 +8964,14 @@
       <c r="M86" t="s">
         <v>548</v>
       </c>
-      <c r="AA86" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="87" spans="1:27">
+      <c r="AA86" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28">
       <c r="A87" t="s">
         <v>558</v>
       </c>
@@ -9160,11 +8987,14 @@
       <c r="M87" t="s">
         <v>548</v>
       </c>
-      <c r="AA87" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="88" spans="1:27">
+      <c r="AA87" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB87" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28">
       <c r="A88" t="s">
         <v>558</v>
       </c>
@@ -9180,11 +9010,14 @@
       <c r="M88" t="s">
         <v>548</v>
       </c>
-      <c r="AA88" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="89" spans="1:27">
+      <c r="AA88" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB88" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28">
       <c r="A89" t="s">
         <v>558</v>
       </c>
@@ -9200,11 +9033,14 @@
       <c r="M89" t="s">
         <v>548</v>
       </c>
-      <c r="AA89" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="90" spans="1:27">
+      <c r="AA89" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB89" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28">
       <c r="A90" t="s">
         <v>558</v>
       </c>
@@ -9220,11 +9056,14 @@
       <c r="M90" t="s">
         <v>548</v>
       </c>
-      <c r="AA90" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="91" spans="1:27">
+      <c r="AA90" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB90" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28">
       <c r="A91" t="s">
         <v>558</v>
       </c>
@@ -9240,11 +9079,14 @@
       <c r="M91" t="s">
         <v>548</v>
       </c>
-      <c r="AA91" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="92" spans="1:27">
+      <c r="AA91" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB91" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28">
       <c r="A92" t="s">
         <v>558</v>
       </c>
@@ -9260,11 +9102,14 @@
       <c r="M92" t="s">
         <v>548</v>
       </c>
-      <c r="AA92" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="93" spans="1:27">
+      <c r="AA92" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB92" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28">
       <c r="A93" t="s">
         <v>558</v>
       </c>
@@ -9280,11 +9125,14 @@
       <c r="M93" t="s">
         <v>548</v>
       </c>
-      <c r="AA93" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="94" spans="1:27">
+      <c r="AA93" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB93" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28">
       <c r="A94" t="s">
         <v>558</v>
       </c>
@@ -9300,11 +9148,14 @@
       <c r="M94" t="s">
         <v>548</v>
       </c>
-      <c r="AA94" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="95" spans="1:27">
+      <c r="AA94" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB94" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28">
       <c r="A95" t="s">
         <v>558</v>
       </c>
@@ -9320,11 +9171,14 @@
       <c r="M95" t="s">
         <v>548</v>
       </c>
-      <c r="AA95" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="96" spans="1:27">
+      <c r="AA95" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB95" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28">
       <c r="A96" t="s">
         <v>558</v>
       </c>
@@ -9340,11 +9194,14 @@
       <c r="M96" t="s">
         <v>548</v>
       </c>
-      <c r="AA96" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="97" spans="1:27">
+      <c r="AA96" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB96" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28">
       <c r="A97" t="s">
         <v>558</v>
       </c>
@@ -9360,11 +9217,14 @@
       <c r="M97" t="s">
         <v>548</v>
       </c>
-      <c r="AA97" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="98" spans="1:27">
+      <c r="AA97" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB97" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28">
       <c r="A98" t="s">
         <v>558</v>
       </c>
@@ -9380,11 +9240,14 @@
       <c r="M98" t="s">
         <v>548</v>
       </c>
-      <c r="AA98" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="99" spans="1:27">
+      <c r="AA98" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB98" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28">
       <c r="A99" t="s">
         <v>558</v>
       </c>
@@ -9400,11 +9263,14 @@
       <c r="M99" t="s">
         <v>548</v>
       </c>
-      <c r="AA99" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="100" spans="1:27">
+      <c r="AA99" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB99" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28">
       <c r="A100" t="s">
         <v>558</v>
       </c>
@@ -9420,11 +9286,14 @@
       <c r="M100" t="s">
         <v>548</v>
       </c>
-      <c r="AA100" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="101" spans="1:27">
+      <c r="AA100" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28">
       <c r="A101" t="s">
         <v>558</v>
       </c>
@@ -9440,11 +9309,14 @@
       <c r="M101" t="s">
         <v>548</v>
       </c>
-      <c r="AA101" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="102" spans="1:27">
+      <c r="AA101" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB101" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28">
       <c r="A102" t="s">
         <v>558</v>
       </c>
@@ -9460,11 +9332,14 @@
       <c r="M102" t="s">
         <v>548</v>
       </c>
-      <c r="AA102" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="103" spans="1:27">
+      <c r="AA102" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB102" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28">
       <c r="A103" t="s">
         <v>558</v>
       </c>
@@ -9480,8 +9355,11 @@
       <c r="M103" t="s">
         <v>548</v>
       </c>
-      <c r="AA103" s="42">
-        <v>43845</v>
+      <c r="AA103" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB103" t="s">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -9554,15 +9432,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
@@ -9570,7 +9448,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>215</v>
       </c>
       <c r="B3" t="s">
@@ -9578,7 +9456,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>217</v>
       </c>
       <c r="B4" t="s">
@@ -9586,7 +9464,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="11" t="s">
         <v>218</v>
       </c>
       <c r="B5" t="s">

</xml_diff>

<commit_message>
EVA-3304 - Validate the presence of the collection location and date (#155)
* Validate the presence of the collection location and date
* Update test
Co-authored-by: April Shen <april.tuesday@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet2.xlsx
+++ b/tests/resources/brokering/metadata_sheet2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48765435-9871-F346-8455-1D9A2A0B4633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CECB4B9-460A-7E49-A573-3736DCAC05D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40240" yWindow="1340" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="767">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2892,19 +2892,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2913,25 +2912,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2940,23 +2931,14 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2966,7 +2948,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2985,8 +2967,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3008,59 +2989,54 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3068,7 +3044,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3426,7 +3402,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AMK23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -3436,208 +3412,216 @@
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="255.5" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.83203125" style="2" customWidth="1"/>
+    <col min="3" max="1025" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="77" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1">
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A3" s="78" t="s">
+      <c r="B2" s="69"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A3" s="70" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="19">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" s="9" customFormat="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" ht="19">
-      <c r="A6" s="7" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1">
+      <c r="A5" s="67"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A6" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="82" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A7" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1">
-      <c r="A8" s="83"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" ht="19">
-      <c r="A9" s="79" t="s">
+      <c r="B7" s="64"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1">
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="19">
+      <c r="A9" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" s="9" customFormat="1">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" s="11" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="84" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1">
+      <c r="A10" s="67"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A11" s="68" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="84"/>
-    </row>
-    <row r="12" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A12" s="35" t="s">
+      <c r="B11" s="68"/>
+    </row>
+    <row r="12" spans="1:8" ht="20">
+      <c r="A12" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A13" s="37" t="s">
+    <row r="13" spans="1:8" ht="20">
+      <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" s="11" customFormat="1" ht="20">
-      <c r="A14" s="38" t="s">
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" ht="20">
+      <c r="A14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="11" customFormat="1" ht="40">
-      <c r="A15" s="39" t="s">
+    <row r="15" spans="1:8" ht="40">
+      <c r="A15" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" ht="40">
-      <c r="A16" s="40" t="s">
+    <row r="16" spans="1:8" ht="40">
+      <c r="A16" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="11" customFormat="1" ht="20">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:2" ht="20">
+      <c r="A17" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="8" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="11" customFormat="1"/>
+    <row r="18" spans="1:2">
+      <c r="A18"/>
+      <c r="B18"/>
+    </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="81"/>
+      <c r="B19" s="63"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="81"/>
+      <c r="B20" s="63"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="81"/>
+      <c r="B21" s="63"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="81"/>
-    </row>
-    <row r="23" spans="1:2" s="4" customFormat="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="B22" s="63"/>
+    </row>
+    <row r="23" spans="1:2" s="3" customFormat="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3647,11 +3631,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3677,16 +3656,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3752,7 +3731,7 @@
   <sheetPr>
     <tabColor rgb="FFB3A2C7"/>
   </sheetPr>
-  <dimension ref="A1:K281"/>
+  <dimension ref="A1:G281"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3768,41 +3747,39 @@
     <col min="8" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="33" customFormat="1">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:7" s="20" customFormat="1">
+      <c r="A1" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>162</v>
       </c>
       <c r="E2" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="18" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>220</v>
       </c>
       <c r="B3" t="s">
@@ -3814,12 +3791,12 @@
       <c r="E3" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="24"/>
       <c r="G3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -3836,7 +3813,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>227</v>
       </c>
@@ -3850,7 +3827,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>230</v>
       </c>
@@ -3864,7 +3841,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>233</v>
       </c>
@@ -3878,7 +3855,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>236</v>
       </c>
@@ -3892,7 +3869,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>240</v>
       </c>
@@ -3906,7 +3883,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -3917,7 +3894,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>244</v>
       </c>
@@ -3928,7 +3905,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>246</v>
       </c>
@@ -3939,7 +3916,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>248</v>
       </c>
@@ -3947,7 +3924,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:7">
       <c r="B14" t="s">
         <v>249</v>
       </c>
@@ -3955,7 +3932,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:7">
       <c r="B15" t="s">
         <v>250</v>
       </c>
@@ -3963,7 +3940,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>251</v>
       </c>
@@ -4111,7 +4088,7 @@
       <c r="B34" t="s">
         <v>269</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4175,7 +4152,7 @@
       <c r="B42" t="s">
         <v>277</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4268,7 +4245,7 @@
       <c r="B54" t="s">
         <v>289</v>
       </c>
-      <c r="E54" s="33"/>
+      <c r="E54" s="20"/>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" t="s">
@@ -5436,26 +5413,26 @@
     <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="64" customFormat="1">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="33" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5466,10 +5443,10 @@
       <c r="B2" t="s">
         <v>761</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="60" t="s">
         <v>762</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="61" t="s">
         <v>763</v>
       </c>
       <c r="E2" t="s">
@@ -5489,10 +5466,10 @@
       <c r="B3" t="s">
         <v>761</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="60" t="s">
         <v>762</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="61" t="s">
         <v>765</v>
       </c>
       <c r="E3" t="s">
@@ -5535,50 +5512,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5618,7 +5595,7 @@
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5655,10 +5632,10 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="14" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5690,62 +5667,62 @@
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="40.5" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="42" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="32" customWidth="1"/>
     <col min="12" max="12" width="64.6640625" customWidth="1"/>
     <col min="13" max="14" width="6" customWidth="1"/>
     <col min="15" max="15" width="6.6640625" customWidth="1"/>
     <col min="16" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="64" customFormat="1">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="37" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="62" t="s">
         <v>553</v>
       </c>
       <c r="B2" t="s">
@@ -5788,15 +5765,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B2" t="s">
@@ -5804,7 +5781,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
@@ -5812,7 +5789,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
@@ -5820,7 +5797,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
@@ -5828,7 +5805,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>162</v>
       </c>
       <c r="B6" t="s">
@@ -5836,7 +5813,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="11" t="s">
         <v>163</v>
       </c>
       <c r="B7" t="s">
@@ -5860,7 +5837,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" t="s">
         <v>168</v>
       </c>
       <c r="B10" t="s">
@@ -5916,7 +5893,7 @@
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="11" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6081,7 +6058,7 @@
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="18" t="s">
+      <c r="A53" t="s">
         <v>187</v>
       </c>
     </row>
@@ -6121,7 +6098,7 @@
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="18" t="s">
+      <c r="A61" t="s">
         <v>191</v>
       </c>
     </row>
@@ -6185,7 +6162,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -6210,56 +6187,55 @@
     <col min="16" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="P1" s="64"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="75" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="62" t="s">
         <v>557</v>
       </c>
       <c r="B2" t="s">
@@ -6268,7 +6244,7 @@
       <c r="C2" t="s">
         <v>559</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="62" t="s">
         <v>553</v>
       </c>
       <c r="E2" t="s">
@@ -6278,7 +6254,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1"/>
+    <row r="3" spans="1:15" ht="15" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="1">
@@ -6318,850 +6294,438 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="2" width="212" style="18" customWidth="1"/>
+    <col min="2" max="2" width="212" customWidth="1"/>
     <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="57" customHeight="1">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:2" ht="57" customHeight="1">
+      <c r="A3" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="16" t="s">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="18"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="25" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="11" t="s">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12">
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" ht="17">
-      <c r="A15" s="25" t="s">
+      <c r="B14" s="16"/>
+    </row>
+    <row r="15" spans="1:2" ht="17">
+      <c r="A15" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="25" t="s">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="11" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="26" t="s">
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="11" t="s">
+      <c r="B18" s="16"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="11" t="s">
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="26" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="11" t="s">
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="11" t="s">
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="11" t="s">
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="11" t="s">
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="11" t="s">
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="26" t="s">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="11" t="s">
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="11" t="s">
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="11" t="s">
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="26" t="s">
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="11" t="s">
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="11" t="s">
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="11" t="s">
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="11" t="s">
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="11" t="s">
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
         <v>115</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="11" t="s">
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="11" t="s">
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="11" t="s">
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="11" t="s">
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:12" ht="51">
-      <c r="A41" s="11" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="51">
+      <c r="A41" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="26" t="s">
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="11" t="s">
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="11" t="s">
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="11" t="s">
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46" s="11" t="s">
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
         <v>134</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="11" t="s">
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
         <v>136</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="11" t="s">
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="11" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="B49" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50" s="11" t="s">
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="11" t="s">
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>144</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="A52" s="11" t="s">
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>146</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" s="26" t="s">
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="1:12" ht="24">
-      <c r="A54" s="30" t="s">
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:2" ht="24">
+      <c r="A54" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-    </row>
-    <row r="55" spans="1:12" ht="15" customHeight="1">
-      <c r="A55" s="31" t="s">
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:2" ht="15" customHeight="1">
+      <c r="A55" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="A56" s="11" t="s">
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="16" t="s">
         <v>152</v>
       </c>
     </row>
@@ -7177,8 +6741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M103" sqref="M103"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7207,7 +6771,7 @@
     <col min="23" max="23" width="11.5" customWidth="1"/>
     <col min="24" max="24" width="15.6640625" customWidth="1"/>
     <col min="25" max="26" width="16.6640625" customWidth="1"/>
-    <col min="27" max="27" width="13.83203125" style="42" customWidth="1"/>
+    <col min="27" max="27" width="13.83203125" style="32" customWidth="1"/>
     <col min="28" max="28" width="34.33203125" customWidth="1"/>
     <col min="29" max="29" width="33.6640625" customWidth="1"/>
     <col min="30" max="30" width="4.6640625" customWidth="1"/>
@@ -7230,256 +6794,256 @@
     <col min="47" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="65" customFormat="1">
-      <c r="A1" s="62"/>
-      <c r="B1" s="86" t="s">
+    <row r="1" spans="1:46">
+      <c r="A1" s="51"/>
+      <c r="B1" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="49" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="68"/>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="69"/>
-    </row>
-    <row r="2" spans="1:46" s="64" customFormat="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="85" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="55"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="55"/>
+      <c r="AG1" s="55"/>
+      <c r="AH1" s="55"/>
+      <c r="AI1" s="55"/>
+      <c r="AJ1" s="55"/>
+      <c r="AK1" s="55"/>
+      <c r="AL1" s="55"/>
+      <c r="AM1" s="55"/>
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="55"/>
+      <c r="AS1" s="55"/>
+      <c r="AT1" s="56"/>
+    </row>
+    <row r="2" spans="1:46">
+      <c r="A2" s="52"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="88" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88" t="s">
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="85" t="s">
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85" t="s">
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="X2" s="85"/>
-      <c r="Y2" s="85"/>
-      <c r="Z2" s="85" t="s">
+      <c r="X2" s="71"/>
+      <c r="Y2" s="71"/>
+      <c r="Z2" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="85"/>
-      <c r="AC2" s="85"/>
-      <c r="AD2" s="85"/>
-      <c r="AE2" s="85"/>
-      <c r="AF2" s="85"/>
-      <c r="AG2" s="85"/>
-      <c r="AH2" s="85"/>
-      <c r="AI2" s="85"/>
-      <c r="AJ2" s="85" t="s">
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="71"/>
+      <c r="AI2" s="71"/>
+      <c r="AJ2" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="AK2" s="85"/>
-      <c r="AL2" s="85"/>
-      <c r="AM2" s="85"/>
-      <c r="AN2" s="85"/>
-      <c r="AO2" s="85"/>
-      <c r="AP2" s="85"/>
-      <c r="AQ2" s="85"/>
-      <c r="AR2" s="85"/>
-      <c r="AS2" s="85"/>
-    </row>
-    <row r="3" spans="1:46" s="64" customFormat="1" ht="26">
-      <c r="A3" s="50" t="s">
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="71"/>
+      <c r="AR2" s="71"/>
+      <c r="AS2" s="71"/>
+    </row>
+    <row r="3" spans="1:46" ht="26">
+      <c r="A3" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="58" t="s">
+      <c r="N3" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="O3" s="57" t="s">
+      <c r="O3" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="P3" s="59" t="s">
+      <c r="P3" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="Q3" s="57" t="s">
+      <c r="Q3" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="R3" s="60" t="s">
+      <c r="R3" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="57" t="s">
+      <c r="S3" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="57" t="s">
+      <c r="T3" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="57" t="s">
+      <c r="U3" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="V3" s="58" t="s">
+      <c r="V3" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="W3" s="60" t="s">
+      <c r="W3" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="X3" s="57" t="s">
+      <c r="X3" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="Y3" s="58" t="s">
+      <c r="Y3" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="Z3" s="60" t="s">
+      <c r="Z3" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="AA3" s="71" t="s">
+      <c r="AA3" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="AB3" s="57" t="s">
+      <c r="AB3" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="57" t="s">
+      <c r="AC3" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="AD3" s="57" t="s">
+      <c r="AD3" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="AE3" s="57" t="s">
+      <c r="AE3" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="AF3" s="57" t="s">
+      <c r="AF3" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="AG3" s="57" t="s">
+      <c r="AG3" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="AH3" s="57" t="s">
+      <c r="AH3" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="AI3" s="58" t="s">
+      <c r="AI3" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="AJ3" s="60" t="s">
+      <c r="AJ3" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="AK3" s="57" t="s">
+      <c r="AK3" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="AL3" s="57" t="s">
+      <c r="AL3" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="AM3" s="57" t="s">
+      <c r="AM3" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="AN3" s="57" t="s">
+      <c r="AN3" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="AO3" s="57" t="s">
+      <c r="AO3" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="AP3" s="57" t="s">
+      <c r="AP3" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="AQ3" s="57" t="s">
+      <c r="AQ3" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="AR3" s="57" t="s">
+      <c r="AR3" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="AS3" s="58" t="s">
+      <c r="AS3" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="AT3" s="61" t="s">
+      <c r="AT3" s="50" t="s">
         <v>148</v>
       </c>
     </row>
@@ -7499,8 +7063,11 @@
       <c r="M4" t="s">
         <v>548</v>
       </c>
-      <c r="AA4" s="42">
-        <v>43845</v>
+      <c r="AA4" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:46">
@@ -7519,8 +7086,11 @@
       <c r="M5" t="s">
         <v>548</v>
       </c>
-      <c r="AA5" s="42">
-        <v>43845</v>
+      <c r="AA5" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:46">
@@ -7539,8 +7109,11 @@
       <c r="M6" t="s">
         <v>548</v>
       </c>
-      <c r="AA6" s="42">
-        <v>43845</v>
+      <c r="AA6" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:46">
@@ -7559,9 +7132,12 @@
       <c r="M7" t="s">
         <v>548</v>
       </c>
-      <c r="Z7" s="72"/>
-      <c r="AA7" s="42">
-        <v>43845</v>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="8" spans="1:46">
@@ -7580,8 +7156,11 @@
       <c r="M8" t="s">
         <v>548</v>
       </c>
-      <c r="AA8" s="42">
-        <v>43845</v>
+      <c r="AA8" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:46">
@@ -7600,8 +7179,11 @@
       <c r="M9" t="s">
         <v>548</v>
       </c>
-      <c r="AA9" s="42">
-        <v>43845</v>
+      <c r="AA9" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="1:46">
@@ -7620,8 +7202,11 @@
       <c r="M10" t="s">
         <v>548</v>
       </c>
-      <c r="AA10" s="42">
-        <v>43845</v>
+      <c r="AA10" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:46">
@@ -7640,8 +7225,11 @@
       <c r="M11" t="s">
         <v>548</v>
       </c>
-      <c r="AA11" s="42">
-        <v>43845</v>
+      <c r="AA11" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:46">
@@ -7660,8 +7248,11 @@
       <c r="M12" t="s">
         <v>548</v>
       </c>
-      <c r="AA12" s="42">
-        <v>43845</v>
+      <c r="AA12" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="13" spans="1:46">
@@ -7680,8 +7271,11 @@
       <c r="M13" t="s">
         <v>548</v>
       </c>
-      <c r="AA13" s="42">
-        <v>43845</v>
+      <c r="AA13" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="14" spans="1:46">
@@ -7700,8 +7294,11 @@
       <c r="M14" t="s">
         <v>548</v>
       </c>
-      <c r="AA14" s="42">
-        <v>43845</v>
+      <c r="AA14" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="15" spans="1:46">
@@ -7720,8 +7317,11 @@
       <c r="M15" t="s">
         <v>548</v>
       </c>
-      <c r="AA15" s="42">
-        <v>43845</v>
+      <c r="AA15" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="16" spans="1:46">
@@ -7740,11 +7340,14 @@
       <c r="M16" t="s">
         <v>548</v>
       </c>
-      <c r="AA16" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
+      <c r="AA16" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
         <v>558</v>
       </c>
@@ -7760,11 +7363,14 @@
       <c r="M17" t="s">
         <v>548</v>
       </c>
-      <c r="AA17" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27">
+      <c r="AA17" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
         <v>558</v>
       </c>
@@ -7780,11 +7386,14 @@
       <c r="M18" t="s">
         <v>548</v>
       </c>
-      <c r="AA18" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27">
+      <c r="AA18" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>558</v>
       </c>
@@ -7800,11 +7409,14 @@
       <c r="M19" t="s">
         <v>548</v>
       </c>
-      <c r="AA19" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+      <c r="AA19" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>558</v>
       </c>
@@ -7820,11 +7432,14 @@
       <c r="M20" t="s">
         <v>548</v>
       </c>
-      <c r="AA20" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
+      <c r="AA20" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>558</v>
       </c>
@@ -7840,11 +7455,14 @@
       <c r="M21" t="s">
         <v>548</v>
       </c>
-      <c r="AA21" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
+      <c r="AA21" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28">
       <c r="A22" t="s">
         <v>558</v>
       </c>
@@ -7860,11 +7478,14 @@
       <c r="M22" t="s">
         <v>548</v>
       </c>
-      <c r="AA22" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
+      <c r="AA22" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28">
       <c r="A23" t="s">
         <v>558</v>
       </c>
@@ -7880,11 +7501,14 @@
       <c r="M23" t="s">
         <v>548</v>
       </c>
-      <c r="AA23" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27">
+      <c r="AA23" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28">
       <c r="A24" t="s">
         <v>558</v>
       </c>
@@ -7900,11 +7524,14 @@
       <c r="M24" t="s">
         <v>548</v>
       </c>
-      <c r="AA24" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
+      <c r="AA24" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28">
       <c r="A25" t="s">
         <v>558</v>
       </c>
@@ -7920,11 +7547,14 @@
       <c r="M25" t="s">
         <v>548</v>
       </c>
-      <c r="AA25" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27">
+      <c r="AA25" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28">
       <c r="A26" t="s">
         <v>558</v>
       </c>
@@ -7940,11 +7570,14 @@
       <c r="M26" t="s">
         <v>548</v>
       </c>
-      <c r="AA26" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27">
+      <c r="AA26" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28">
       <c r="A27" t="s">
         <v>558</v>
       </c>
@@ -7960,11 +7593,14 @@
       <c r="M27" t="s">
         <v>548</v>
       </c>
-      <c r="AA27" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27">
+      <c r="AA27" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28">
       <c r="A28" t="s">
         <v>558</v>
       </c>
@@ -7980,11 +7616,14 @@
       <c r="M28" t="s">
         <v>548</v>
       </c>
-      <c r="AA28" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27">
+      <c r="AA28" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
       <c r="A29" t="s">
         <v>558</v>
       </c>
@@ -8000,11 +7639,14 @@
       <c r="M29" t="s">
         <v>548</v>
       </c>
-      <c r="AA29" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27">
+      <c r="AA29" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28">
       <c r="A30" t="s">
         <v>558</v>
       </c>
@@ -8020,11 +7662,14 @@
       <c r="M30" t="s">
         <v>548</v>
       </c>
-      <c r="AA30" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27">
+      <c r="AA30" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28">
       <c r="A31" t="s">
         <v>558</v>
       </c>
@@ -8040,11 +7685,14 @@
       <c r="M31" t="s">
         <v>548</v>
       </c>
-      <c r="AA31" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27">
+      <c r="AA31" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28">
       <c r="A32" t="s">
         <v>558</v>
       </c>
@@ -8060,11 +7708,14 @@
       <c r="M32" t="s">
         <v>548</v>
       </c>
-      <c r="AA32" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27">
+      <c r="AA32" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28">
       <c r="A33" t="s">
         <v>558</v>
       </c>
@@ -8080,11 +7731,14 @@
       <c r="M33" t="s">
         <v>548</v>
       </c>
-      <c r="AA33" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27">
+      <c r="AA33" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28">
       <c r="A34" t="s">
         <v>558</v>
       </c>
@@ -8100,11 +7754,14 @@
       <c r="M34" t="s">
         <v>548</v>
       </c>
-      <c r="AA34" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
+      <c r="AA34" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28">
       <c r="A35" t="s">
         <v>558</v>
       </c>
@@ -8120,11 +7777,14 @@
       <c r="M35" t="s">
         <v>548</v>
       </c>
-      <c r="AA35" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27">
+      <c r="AA35" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28">
       <c r="A36" t="s">
         <v>558</v>
       </c>
@@ -8140,11 +7800,14 @@
       <c r="M36" t="s">
         <v>548</v>
       </c>
-      <c r="AA36" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27">
+      <c r="AA36" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28">
       <c r="A37" t="s">
         <v>558</v>
       </c>
@@ -8160,11 +7823,14 @@
       <c r="M37" t="s">
         <v>548</v>
       </c>
-      <c r="AA37" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27">
+      <c r="AA37" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28">
       <c r="A38" t="s">
         <v>558</v>
       </c>
@@ -8180,11 +7846,14 @@
       <c r="M38" t="s">
         <v>548</v>
       </c>
-      <c r="AA38" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27">
+      <c r="AA38" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28">
       <c r="A39" t="s">
         <v>558</v>
       </c>
@@ -8200,11 +7869,14 @@
       <c r="M39" t="s">
         <v>548</v>
       </c>
-      <c r="AA39" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27">
+      <c r="AA39" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28">
       <c r="A40" t="s">
         <v>558</v>
       </c>
@@ -8220,11 +7892,14 @@
       <c r="M40" t="s">
         <v>548</v>
       </c>
-      <c r="AA40" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27">
+      <c r="AA40" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
       <c r="A41" t="s">
         <v>558</v>
       </c>
@@ -8240,11 +7915,14 @@
       <c r="M41" t="s">
         <v>548</v>
       </c>
-      <c r="AA41" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27">
+      <c r="AA41" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28">
       <c r="A42" t="s">
         <v>558</v>
       </c>
@@ -8260,11 +7938,14 @@
       <c r="M42" t="s">
         <v>548</v>
       </c>
-      <c r="AA42" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27">
+      <c r="AA42" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
       <c r="A43" t="s">
         <v>558</v>
       </c>
@@ -8280,11 +7961,14 @@
       <c r="M43" t="s">
         <v>548</v>
       </c>
-      <c r="AA43" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27">
+      <c r="AA43" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
       <c r="A44" t="s">
         <v>558</v>
       </c>
@@ -8300,11 +7984,14 @@
       <c r="M44" t="s">
         <v>548</v>
       </c>
-      <c r="AA44" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27">
+      <c r="AA44" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
       <c r="A45" t="s">
         <v>558</v>
       </c>
@@ -8320,11 +8007,14 @@
       <c r="M45" t="s">
         <v>548</v>
       </c>
-      <c r="AA45" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27">
+      <c r="AA45" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
       <c r="A46" t="s">
         <v>558</v>
       </c>
@@ -8340,11 +8030,14 @@
       <c r="M46" t="s">
         <v>548</v>
       </c>
-      <c r="AA46" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27">
+      <c r="AA46" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
       <c r="A47" t="s">
         <v>558</v>
       </c>
@@ -8360,11 +8053,14 @@
       <c r="M47" t="s">
         <v>548</v>
       </c>
-      <c r="AA47" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27">
+      <c r="AA47" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28">
       <c r="A48" t="s">
         <v>558</v>
       </c>
@@ -8380,11 +8076,14 @@
       <c r="M48" t="s">
         <v>548</v>
       </c>
-      <c r="AA48" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27">
+      <c r="AA48" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28">
       <c r="A49" t="s">
         <v>558</v>
       </c>
@@ -8400,11 +8099,14 @@
       <c r="M49" t="s">
         <v>548</v>
       </c>
-      <c r="AA49" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27">
+      <c r="AA49" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28">
       <c r="A50" t="s">
         <v>558</v>
       </c>
@@ -8420,11 +8122,14 @@
       <c r="M50" t="s">
         <v>548</v>
       </c>
-      <c r="AA50" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="51" spans="1:27">
+      <c r="AA50" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28">
       <c r="A51" t="s">
         <v>558</v>
       </c>
@@ -8440,11 +8145,14 @@
       <c r="M51" t="s">
         <v>548</v>
       </c>
-      <c r="AA51" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="52" spans="1:27">
+      <c r="AA51" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28">
       <c r="A52" t="s">
         <v>558</v>
       </c>
@@ -8460,11 +8168,14 @@
       <c r="M52" t="s">
         <v>548</v>
       </c>
-      <c r="AA52" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="53" spans="1:27">
+      <c r="AA52" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28">
       <c r="A53" t="s">
         <v>558</v>
       </c>
@@ -8480,11 +8191,14 @@
       <c r="M53" t="s">
         <v>548</v>
       </c>
-      <c r="AA53" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="54" spans="1:27">
+      <c r="AA53" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28">
       <c r="A54" t="s">
         <v>558</v>
       </c>
@@ -8500,11 +8214,14 @@
       <c r="M54" t="s">
         <v>548</v>
       </c>
-      <c r="AA54" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="55" spans="1:27">
+      <c r="AA54" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28">
       <c r="A55" t="s">
         <v>558</v>
       </c>
@@ -8520,11 +8237,14 @@
       <c r="M55" t="s">
         <v>548</v>
       </c>
-      <c r="AA55" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="56" spans="1:27">
+      <c r="AA55" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28">
       <c r="A56" t="s">
         <v>558</v>
       </c>
@@ -8540,11 +8260,14 @@
       <c r="M56" t="s">
         <v>548</v>
       </c>
-      <c r="AA56" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27">
+      <c r="AA56" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28">
       <c r="A57" t="s">
         <v>558</v>
       </c>
@@ -8560,11 +8283,14 @@
       <c r="M57" t="s">
         <v>548</v>
       </c>
-      <c r="AA57" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="58" spans="1:27">
+      <c r="AA57" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28">
       <c r="A58" t="s">
         <v>558</v>
       </c>
@@ -8580,11 +8306,14 @@
       <c r="M58" t="s">
         <v>548</v>
       </c>
-      <c r="AA58" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27">
+      <c r="AA58" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28">
       <c r="A59" t="s">
         <v>558</v>
       </c>
@@ -8600,11 +8329,14 @@
       <c r="M59" t="s">
         <v>548</v>
       </c>
-      <c r="AA59" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27">
+      <c r="AA59" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28">
       <c r="A60" t="s">
         <v>558</v>
       </c>
@@ -8620,11 +8352,14 @@
       <c r="M60" t="s">
         <v>548</v>
       </c>
-      <c r="AA60" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27">
+      <c r="AA60" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28">
       <c r="A61" t="s">
         <v>558</v>
       </c>
@@ -8640,11 +8375,14 @@
       <c r="M61" t="s">
         <v>548</v>
       </c>
-      <c r="AA61" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27">
+      <c r="AA61" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28">
       <c r="A62" t="s">
         <v>558</v>
       </c>
@@ -8660,11 +8398,14 @@
       <c r="M62" t="s">
         <v>548</v>
       </c>
-      <c r="AA62" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="63" spans="1:27">
+      <c r="AA62" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28">
       <c r="A63" t="s">
         <v>558</v>
       </c>
@@ -8680,11 +8421,14 @@
       <c r="M63" t="s">
         <v>548</v>
       </c>
-      <c r="AA63" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="64" spans="1:27">
+      <c r="AA63" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28">
       <c r="A64" t="s">
         <v>558</v>
       </c>
@@ -8700,11 +8444,14 @@
       <c r="M64" t="s">
         <v>548</v>
       </c>
-      <c r="AA64" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="65" spans="1:27">
+      <c r="AA64" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28">
       <c r="A65" t="s">
         <v>558</v>
       </c>
@@ -8720,11 +8467,14 @@
       <c r="M65" t="s">
         <v>548</v>
       </c>
-      <c r="AA65" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="66" spans="1:27">
+      <c r="AA65" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28">
       <c r="A66" t="s">
         <v>558</v>
       </c>
@@ -8740,11 +8490,14 @@
       <c r="M66" t="s">
         <v>548</v>
       </c>
-      <c r="AA66" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="67" spans="1:27">
+      <c r="AA66" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28">
       <c r="A67" t="s">
         <v>558</v>
       </c>
@@ -8760,11 +8513,14 @@
       <c r="M67" t="s">
         <v>548</v>
       </c>
-      <c r="AA67" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="68" spans="1:27">
+      <c r="AA67" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28">
       <c r="A68" t="s">
         <v>558</v>
       </c>
@@ -8780,11 +8536,14 @@
       <c r="M68" t="s">
         <v>548</v>
       </c>
-      <c r="AA68" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="69" spans="1:27">
+      <c r="AA68" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28">
       <c r="A69" t="s">
         <v>558</v>
       </c>
@@ -8800,11 +8559,14 @@
       <c r="M69" t="s">
         <v>548</v>
       </c>
-      <c r="AA69" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="70" spans="1:27">
+      <c r="AA69" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28">
       <c r="A70" t="s">
         <v>558</v>
       </c>
@@ -8820,11 +8582,14 @@
       <c r="M70" t="s">
         <v>548</v>
       </c>
-      <c r="AA70" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="71" spans="1:27">
+      <c r="AA70" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28">
       <c r="A71" t="s">
         <v>558</v>
       </c>
@@ -8840,11 +8605,14 @@
       <c r="M71" t="s">
         <v>548</v>
       </c>
-      <c r="AA71" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="72" spans="1:27">
+      <c r="AA71" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28">
       <c r="A72" t="s">
         <v>558</v>
       </c>
@@ -8860,11 +8628,14 @@
       <c r="M72" t="s">
         <v>548</v>
       </c>
-      <c r="AA72" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="73" spans="1:27">
+      <c r="AA72" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28">
       <c r="A73" t="s">
         <v>558</v>
       </c>
@@ -8880,11 +8651,14 @@
       <c r="M73" t="s">
         <v>548</v>
       </c>
-      <c r="AA73" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="74" spans="1:27">
+      <c r="AA73" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28">
       <c r="A74" t="s">
         <v>558</v>
       </c>
@@ -8900,11 +8674,14 @@
       <c r="M74" t="s">
         <v>548</v>
       </c>
-      <c r="AA74" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="75" spans="1:27">
+      <c r="AA74" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28">
       <c r="A75" t="s">
         <v>558</v>
       </c>
@@ -8920,11 +8697,14 @@
       <c r="M75" t="s">
         <v>548</v>
       </c>
-      <c r="AA75" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="76" spans="1:27">
+      <c r="AA75" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28">
       <c r="A76" t="s">
         <v>558</v>
       </c>
@@ -8940,11 +8720,14 @@
       <c r="M76" t="s">
         <v>548</v>
       </c>
-      <c r="AA76" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="77" spans="1:27">
+      <c r="AA76" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28">
       <c r="A77" t="s">
         <v>558</v>
       </c>
@@ -8960,11 +8743,14 @@
       <c r="M77" t="s">
         <v>548</v>
       </c>
-      <c r="AA77" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="78" spans="1:27">
+      <c r="AA77" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28">
       <c r="A78" t="s">
         <v>558</v>
       </c>
@@ -8980,11 +8766,14 @@
       <c r="M78" t="s">
         <v>548</v>
       </c>
-      <c r="AA78" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="79" spans="1:27">
+      <c r="AA78" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28">
       <c r="A79" t="s">
         <v>558</v>
       </c>
@@ -9000,11 +8789,14 @@
       <c r="M79" t="s">
         <v>548</v>
       </c>
-      <c r="AA79" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="80" spans="1:27">
+      <c r="AA79" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28">
       <c r="A80" t="s">
         <v>558</v>
       </c>
@@ -9020,11 +8812,14 @@
       <c r="M80" t="s">
         <v>548</v>
       </c>
-      <c r="AA80" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="81" spans="1:27">
+      <c r="AA80" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28">
       <c r="A81" t="s">
         <v>558</v>
       </c>
@@ -9040,11 +8835,14 @@
       <c r="M81" t="s">
         <v>548</v>
       </c>
-      <c r="AA81" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="82" spans="1:27">
+      <c r="AA81" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28">
       <c r="A82" t="s">
         <v>558</v>
       </c>
@@ -9060,11 +8858,14 @@
       <c r="M82" t="s">
         <v>548</v>
       </c>
-      <c r="AA82" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="83" spans="1:27">
+      <c r="AA82" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28">
       <c r="A83" t="s">
         <v>558</v>
       </c>
@@ -9080,11 +8881,14 @@
       <c r="M83" t="s">
         <v>548</v>
       </c>
-      <c r="AA83" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="84" spans="1:27">
+      <c r="AA83" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28">
       <c r="A84" t="s">
         <v>558</v>
       </c>
@@ -9100,11 +8904,14 @@
       <c r="M84" t="s">
         <v>548</v>
       </c>
-      <c r="AA84" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="85" spans="1:27">
+      <c r="AA84" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28">
       <c r="A85" t="s">
         <v>558</v>
       </c>
@@ -9120,11 +8927,14 @@
       <c r="M85" t="s">
         <v>548</v>
       </c>
-      <c r="AA85" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="86" spans="1:27">
+      <c r="AA85" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28">
       <c r="A86" t="s">
         <v>558</v>
       </c>
@@ -9140,11 +8950,14 @@
       <c r="M86" t="s">
         <v>548</v>
       </c>
-      <c r="AA86" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="87" spans="1:27">
+      <c r="AA86" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28">
       <c r="A87" t="s">
         <v>558</v>
       </c>
@@ -9160,11 +8973,14 @@
       <c r="M87" t="s">
         <v>548</v>
       </c>
-      <c r="AA87" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="88" spans="1:27">
+      <c r="AA87" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB87" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28">
       <c r="A88" t="s">
         <v>558</v>
       </c>
@@ -9180,11 +8996,14 @@
       <c r="M88" t="s">
         <v>548</v>
       </c>
-      <c r="AA88" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="89" spans="1:27">
+      <c r="AA88" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB88" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28">
       <c r="A89" t="s">
         <v>558</v>
       </c>
@@ -9200,11 +9019,14 @@
       <c r="M89" t="s">
         <v>548</v>
       </c>
-      <c r="AA89" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="90" spans="1:27">
+      <c r="AA89" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB89" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28">
       <c r="A90" t="s">
         <v>558</v>
       </c>
@@ -9220,11 +9042,14 @@
       <c r="M90" t="s">
         <v>548</v>
       </c>
-      <c r="AA90" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="91" spans="1:27">
+      <c r="AA90" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB90" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28">
       <c r="A91" t="s">
         <v>558</v>
       </c>
@@ -9240,11 +9065,14 @@
       <c r="M91" t="s">
         <v>548</v>
       </c>
-      <c r="AA91" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="92" spans="1:27">
+      <c r="AA91" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB91" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28">
       <c r="A92" t="s">
         <v>558</v>
       </c>
@@ -9260,11 +9088,14 @@
       <c r="M92" t="s">
         <v>548</v>
       </c>
-      <c r="AA92" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="93" spans="1:27">
+      <c r="AA92" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB92" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28">
       <c r="A93" t="s">
         <v>558</v>
       </c>
@@ -9280,11 +9111,14 @@
       <c r="M93" t="s">
         <v>548</v>
       </c>
-      <c r="AA93" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="94" spans="1:27">
+      <c r="AA93" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB93" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28">
       <c r="A94" t="s">
         <v>558</v>
       </c>
@@ -9300,11 +9134,14 @@
       <c r="M94" t="s">
         <v>548</v>
       </c>
-      <c r="AA94" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="95" spans="1:27">
+      <c r="AA94" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB94" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28">
       <c r="A95" t="s">
         <v>558</v>
       </c>
@@ -9320,11 +9157,14 @@
       <c r="M95" t="s">
         <v>548</v>
       </c>
-      <c r="AA95" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="96" spans="1:27">
+      <c r="AA95" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB95" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28">
       <c r="A96" t="s">
         <v>558</v>
       </c>
@@ -9340,11 +9180,14 @@
       <c r="M96" t="s">
         <v>548</v>
       </c>
-      <c r="AA96" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="97" spans="1:27">
+      <c r="AA96" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB96" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28">
       <c r="A97" t="s">
         <v>558</v>
       </c>
@@ -9360,11 +9203,14 @@
       <c r="M97" t="s">
         <v>548</v>
       </c>
-      <c r="AA97" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="98" spans="1:27">
+      <c r="AA97" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB97" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28">
       <c r="A98" t="s">
         <v>558</v>
       </c>
@@ -9380,11 +9226,14 @@
       <c r="M98" t="s">
         <v>548</v>
       </c>
-      <c r="AA98" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="99" spans="1:27">
+      <c r="AA98" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB98" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28">
       <c r="A99" t="s">
         <v>558</v>
       </c>
@@ -9400,11 +9249,14 @@
       <c r="M99" t="s">
         <v>548</v>
       </c>
-      <c r="AA99" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="100" spans="1:27">
+      <c r="AA99" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB99" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28">
       <c r="A100" t="s">
         <v>558</v>
       </c>
@@ -9420,11 +9272,14 @@
       <c r="M100" t="s">
         <v>548</v>
       </c>
-      <c r="AA100" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="101" spans="1:27">
+      <c r="AA100" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28">
       <c r="A101" t="s">
         <v>558</v>
       </c>
@@ -9440,11 +9295,14 @@
       <c r="M101" t="s">
         <v>548</v>
       </c>
-      <c r="AA101" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="102" spans="1:27">
+      <c r="AA101" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB101" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28">
       <c r="A102" t="s">
         <v>558</v>
       </c>
@@ -9460,11 +9318,14 @@
       <c r="M102" t="s">
         <v>548</v>
       </c>
-      <c r="AA102" s="42">
-        <v>43845</v>
-      </c>
-    </row>
-    <row r="103" spans="1:27">
+      <c r="AA102" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB102" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28">
       <c r="A103" t="s">
         <v>558</v>
       </c>
@@ -9480,8 +9341,11 @@
       <c r="M103" t="s">
         <v>548</v>
       </c>
-      <c r="AA103" s="42">
-        <v>43845</v>
+      <c r="AA103" s="32">
+        <v>43845</v>
+      </c>
+      <c r="AB103" t="s">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -9554,15 +9418,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
@@ -9570,7 +9434,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>215</v>
       </c>
       <c r="B3" t="s">
@@ -9578,7 +9442,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>217</v>
       </c>
       <c r="B4" t="s">
@@ -9586,7 +9450,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="11" t="s">
         <v>218</v>
       </c>
       <c r="B5" t="s">

</xml_diff>

<commit_message>
Allow hyphens and dots in the novel attributes label and text
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet2.xlsx
+++ b/tests/resources/brokering/metadata_sheet2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CECB4B9-460A-7E49-A573-3736DCAC05D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD57FF9-F129-5B42-9733-7DFBBE0A4553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40240" yWindow="1340" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33580" yWindow="4020" windowWidth="35840" windowHeight="21100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Files" sheetId="10" r:id="rId10"/>
     <sheet name="CVs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="768">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2480,6 +2480,9 @@
   </si>
   <si>
     <t>TPTB</t>
+  </si>
+  <si>
+    <t>family:168, Label:576-168-1-1, tree.ind:168-B1-R1</t>
   </si>
 </sst>
 </file>
@@ -6741,8 +6744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL10" sqref="AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7068,6 +7071,9 @@
       </c>
       <c r="AB4" t="s">
         <v>515</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="5" spans="1:46">

</xml_diff>

<commit_message>
Improve novel attributes validation (#176)
* Allow hyphens and dots in the novel attributes label and text
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet2.xlsx
+++ b/tests/resources/brokering/metadata_sheet2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CECB4B9-460A-7E49-A573-3736DCAC05D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD57FF9-F129-5B42-9733-7DFBBE0A4553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40240" yWindow="1340" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33580" yWindow="4020" windowWidth="35840" windowHeight="21100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Files" sheetId="10" r:id="rId10"/>
     <sheet name="CVs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="768">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2480,6 +2480,9 @@
   </si>
   <si>
     <t>TPTB</t>
+  </si>
+  <si>
+    <t>family:168, Label:576-168-1-1, tree.ind:168-B1-R1</t>
   </si>
 </sst>
 </file>
@@ -6741,8 +6744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL10" sqref="AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7068,6 +7071,9 @@
       </c>
       <c r="AB4" t="s">
         <v>515</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="5" spans="1:46">

</xml_diff>